<commit_message>
Update Detailed run sheet optimization
</commit_message>
<xml_diff>
--- a/Data/Real/DES - Clarity Dental.xlsx
+++ b/Data/Real/DES - Clarity Dental.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\radika\AI_Engineer\Project\Dental_Clinic\Code\Data\Real\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87B014C-BB04-4F28-BFF8-45F8BC1C46A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2677DD9-CD32-4A2C-8430-2129834F6D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -682,7 +682,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -699,6 +699,7 @@
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -917,10 +918,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R166"/>
+  <dimension ref="A1:R167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7096,6 +7097,12 @@
       <c r="I166" s="2">
         <f t="shared" si="2"/>
         <v>2.4948232417733211E-5</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I167" s="10">
+        <f>SUM(I2:I166)</f>
+        <v>0.999999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add run sheet scheduling V3
</commit_message>
<xml_diff>
--- a/Data/Real/DES - Clarity Dental.xlsx
+++ b/Data/Real/DES - Clarity Dental.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\radika\AI_Engineer\Project\Dental_Clinic\Code\Data\Real\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2677DD9-CD32-4A2C-8430-2129834F6D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079B172E-5D32-4D8E-9C21-2614E0331387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model_Input" sheetId="1" r:id="rId1"/>
@@ -921,7 +921,7 @@
   <dimension ref="A1:R167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -937,7 +937,7 @@
     <col min="14" max="14" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="str">
         <f>'Summary Qty'!A1</f>
         <v>Code</v>
@@ -967,7 +967,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f>'Summary Qty'!A2</f>
         <v>11</v>
@@ -1004,7 +1004,7 @@
         <v>3.8619863782651011E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>'Summary Qty'!A3</f>
         <v>12</v>
@@ -1041,7 +1041,7 @@
         <v>5.7031659306938126E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f>'Summary Qty'!A4</f>
         <v>13</v>
@@ -1078,7 +1078,7 @@
         <v>2.6195644038619875E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f>'Summary Qty'!A5</f>
         <v>14</v>
@@ -1121,7 +1121,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>'Summary Qty'!A6</f>
         <v>22</v>
@@ -1167,7 +1167,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f>'Summary Qty'!A7</f>
         <v>24</v>
@@ -1210,7 +1210,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f>'Summary Qty'!A8</f>
         <v>37</v>
@@ -1250,7 +1250,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f>'Summary Qty'!A9</f>
         <v>61</v>
@@ -1287,7 +1287,7 @@
         <v>9.7298106429159531E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f>'Summary Qty'!A10</f>
         <v>71</v>
@@ -1324,7 +1324,7 @@
         <v>1.7463762692413248E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f>'Summary Qty'!A11</f>
         <v>72</v>
@@ -1361,7 +1361,7 @@
         <v>2.8890053139735056E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f>'Summary Qty'!A12</f>
         <v>73</v>
@@ -1398,7 +1398,7 @@
         <v>5.4886111319013065E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f>'Summary Qty'!A13</f>
         <v>74</v>
@@ -1438,7 +1438,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f>'Summary Qty'!A14</f>
         <v>82</v>
@@ -1475,7 +1475,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f>'Summary Qty'!A15</f>
         <v>88011</v>
@@ -1512,7 +1512,7 @@
         <v>7.7589002819150286E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f>'Summary Qty'!A16</f>
         <v>88012</v>
@@ -1549,7 +1549,7 @@
         <v>8.3327096275228937E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f>'Summary Qty'!A17</f>
         <v>88013</v>
@@ -1586,7 +1586,7 @@
         <v>2.6445126362797207E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f>'Summary Qty'!A18</f>
         <v>88022</v>
@@ -1623,7 +1623,7 @@
         <v>1.4145647780854731E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="str">
         <f>'Summary Qty'!A19</f>
         <v>CC</v>
@@ -1660,7 +1660,7 @@
         <v>7.4844697253199639E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f>'Summary Qty'!A20</f>
         <v>111</v>
@@ -1697,7 +1697,7 @@
         <v>1.4968939450639928E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f>'Summary Qty'!A21</f>
         <v>113</v>
@@ -1734,7 +1734,7 @@
         <v>6.2620063368510363E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f>'Summary Qty'!A22</f>
         <v>114</v>
@@ -1771,7 +1771,7 @@
         <v>0.10206321882094657</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f>'Summary Qty'!A23</f>
         <v>115</v>
@@ -1808,7 +1808,7 @@
         <v>3.3680113763939834E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f>'Summary Qty'!A24</f>
         <v>116</v>
@@ -1845,7 +1845,7 @@
         <v>7.4844697253199639E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f>'Summary Qty'!A25</f>
         <v>117</v>
@@ -1882,7 +1882,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f>'Summary Qty'!A26</f>
         <v>118</v>
@@ -1919,7 +1919,7 @@
         <v>1.8386847291869377E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f>'Summary Qty'!A27</f>
         <v>119</v>
@@ -1956,7 +1956,7 @@
         <v>5.6881969912431721E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f>'Summary Qty'!A28</f>
         <v>121</v>
@@ -1993,7 +1993,7 @@
         <v>0.10031684255170524</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f>'Summary Qty'!A29</f>
         <v>123</v>
@@ -2030,7 +2030,7 @@
         <v>4.4906818351919784E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f>'Summary Qty'!A30</f>
         <v>141</v>
@@ -2067,7 +2067,7 @@
         <v>9.9792929670932843E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f>'Summary Qty'!A31</f>
         <v>151</v>
@@ -2104,7 +2104,7 @@
         <v>8.4823990220292921E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f>'Summary Qty'!A32</f>
         <v>161</v>
@@ -2141,7 +2141,7 @@
         <v>2.9189431928747858E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f>'Summary Qty'!A33</f>
         <v>171</v>
@@ -2178,7 +2178,7 @@
         <v>1.671531571988125E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f>'Summary Qty'!A34</f>
         <v>88111</v>
@@ -2215,7 +2215,7 @@
         <v>2.2453409175959892E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f>'Summary Qty'!A35</f>
         <v>88114</v>
@@ -2252,7 +2252,7 @@
         <v>1.2748546765461671E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <f>'Summary Qty'!A36</f>
         <v>88115</v>
@@ -2289,7 +2289,7 @@
         <v>9.9792929670932843E-5</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f>'Summary Qty'!A37</f>
         <v>88121</v>
@@ -2326,7 +2326,7 @@
         <v>1.3372252575905E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <f>'Summary Qty'!A38</f>
         <v>88161</v>
@@ -2363,7 +2363,7 @@
         <v>2.7443055659506534E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f>'Summary Qty'!A39</f>
         <v>88162</v>
@@ -2400,7 +2400,7 @@
         <v>3.2432702143053173E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <f>'Summary Qty'!A40</f>
         <v>213</v>
@@ -2437,7 +2437,7 @@
         <v>4.4906818351919784E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f>'Summary Qty'!A41</f>
         <v>221</v>
@@ -2474,7 +2474,7 @@
         <v>5.2141805753062416E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f>'Summary Qty'!A42</f>
         <v>222</v>
@@ -2511,7 +2511,7 @@
         <v>1.1625876306663676E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <f>'Summary Qty'!A43</f>
         <v>231</v>
@@ -2548,7 +2548,7 @@
         <v>1.3472045505575933E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <f>'Summary Qty'!A44</f>
         <v>250</v>
@@ -2585,7 +2585,7 @@
         <v>5.0395429483821082E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <f>'Summary Qty'!A45</f>
         <v>251</v>
@@ -2622,7 +2622,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <f>'Summary Qty'!A46</f>
         <v>311</v>
@@ -2659,7 +2659,7 @@
         <v>2.2154030386947091E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <f>'Summary Qty'!A47</f>
         <v>314</v>
@@ -2696,7 +2696,7 @@
         <v>2.3201856148491887E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <f>'Summary Qty'!A48</f>
         <v>322</v>
@@ -2733,7 +2733,7 @@
         <v>1.1975151560511942E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <f>'Summary Qty'!A49</f>
         <v>323</v>
@@ -2770,7 +2770,7 @@
         <v>9.4803283187386202E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <f>'Summary Qty'!A50</f>
         <v>324</v>
@@ -2807,7 +2807,7 @@
         <v>2.0457550582541235E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <f>'Summary Qty'!A51</f>
         <v>391</v>
@@ -2844,7 +2844,7 @@
         <v>1.4968939450639928E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <f>'Summary Qty'!A52</f>
         <v>88311</v>
@@ -2881,7 +2881,7 @@
         <v>9.9792929670932838E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <f>'Summary Qty'!A53</f>
         <v>88314</v>
@@ -2918,7 +2918,7 @@
         <v>9.9792929670932843E-5</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <f>'Summary Qty'!A54</f>
         <v>88316</v>
@@ -2955,7 +2955,7 @@
         <v>3.2432702143053173E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <f>'Summary Qty'!A55</f>
         <v>88324</v>
@@ -2992,7 +2992,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <f>'Summary Qty'!A56</f>
         <v>411</v>
@@ -3029,7 +3029,7 @@
         <v>2.9937878901279856E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <f>'Summary Qty'!A57</f>
         <v>414</v>
@@ -3066,7 +3066,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <f>'Summary Qty'!A58</f>
         <v>415</v>
@@ -3103,7 +3103,7 @@
         <v>1.4968939450639928E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <f>'Summary Qty'!A59</f>
         <v>416</v>
@@ -3140,7 +3140,7 @@
         <v>1.5467904098994591E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <f>'Summary Qty'!A60</f>
         <v>417</v>
@@ -3177,7 +3177,7 @@
         <v>1.4719457126462594E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <f>'Summary Qty'!A61</f>
         <v>418</v>
@@ -3214,7 +3214,7 @@
         <v>1.4719457126462594E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <f>'Summary Qty'!A62</f>
         <v>419</v>
@@ -3251,7 +3251,7 @@
         <v>1.8461691989122579E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <f>'Summary Qty'!A63</f>
         <v>431</v>
@@ -3288,7 +3288,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <f>'Summary Qty'!A64</f>
         <v>455</v>
@@ -3325,7 +3325,7 @@
         <v>4.4906818351919784E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <f>'Summary Qty'!A65</f>
         <v>88414</v>
@@ -3362,7 +3362,7 @@
         <v>7.4844697253199639E-5</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <f>'Summary Qty'!A66</f>
         <v>521</v>
@@ -3399,7 +3399,7 @@
         <v>3.34306314397625E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <f>'Summary Qty'!A67</f>
         <v>522</v>
@@ -3436,7 +3436,7 @@
         <v>3.0187361225457185E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <f>'Summary Qty'!A68</f>
         <v>523</v>
@@ -3473,7 +3473,7 @@
         <v>5.8378863857495716E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <f>'Summary Qty'!A69</f>
         <v>524</v>
@@ -3510,7 +3510,7 @@
         <v>5.4387146670658408E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <f>'Summary Qty'!A70</f>
         <v>525</v>
@@ -3547,7 +3547,7 @@
         <v>3.4179078412294498E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <f>'Summary Qty'!A71</f>
         <v>526</v>
@@ -3584,7 +3584,7 @@
         <v>6.7360227527879664E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <f>'Summary Qty'!A72</f>
         <v>531</v>
@@ -3621,7 +3621,7 @@
         <v>1.6141506374273386E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <f>'Summary Qty'!A73</f>
         <v>532</v>
@@ -3658,7 +3658,7 @@
         <v>3.2283012748546773E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <f>'Summary Qty'!A74</f>
         <v>533</v>
@@ -3695,7 +3695,7 @@
         <v>2.4474216001796278E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <f>'Summary Qty'!A75</f>
         <v>534</v>
@@ -3732,7 +3732,7 @@
         <v>1.3172666716563135E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <f>'Summary Qty'!A76</f>
         <v>535</v>
@@ -3769,7 +3769,7 @@
         <v>5.3888182022303732E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <f>'Summary Qty'!A77</f>
         <v>572</v>
@@ -3806,7 +3806,7 @@
         <v>8.9813636703839567E-4</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <f>'Summary Qty'!A78</f>
         <v>574</v>
@@ -3843,7 +3843,7 @@
         <v>1.7463762692413248E-4</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <f>'Summary Qty'!A79</f>
         <v>576</v>
@@ -3880,7 +3880,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <f>'Summary Qty'!A80</f>
         <v>577</v>
@@ -3917,7 +3917,7 @@
         <v>1.4295337175361128E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <f>'Summary Qty'!A81</f>
         <v>578</v>
@@ -3954,7 +3954,7 @@
         <v>2.3201856148491887E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <f>'Summary Qty'!A82</f>
         <v>88521</v>
@@ -3991,7 +3991,7 @@
         <v>1.4968939450639928E-4</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <f>'Summary Qty'!A83</f>
         <v>88523</v>
@@ -4028,7 +4028,7 @@
         <v>1.2474116208866605E-4</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <f>'Summary Qty'!A84</f>
         <v>88524</v>
@@ -4065,7 +4065,7 @@
         <v>1.9958585934186569E-4</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <f>'Summary Qty'!A85</f>
         <v>88525</v>
@@ -4102,7 +4102,7 @@
         <v>9.9792929670932843E-5</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <f>'Summary Qty'!A86</f>
         <v>88531</v>
@@ -4139,7 +4139,7 @@
         <v>1.3721527829753267E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <f>'Summary Qty'!A87</f>
         <v>88532</v>
@@ -4176,7 +4176,7 @@
         <v>4.11645834892598E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <f>'Summary Qty'!A88</f>
         <v>88533</v>
@@ -4213,7 +4213,7 @@
         <v>1.272359853304394E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <f>'Summary Qty'!A89</f>
         <v>88534</v>
@@ -4250,7 +4250,7 @@
         <v>2.2453409175959892E-4</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <f>'Summary Qty'!A90</f>
         <v>88586</v>
@@ -4287,7 +4287,7 @@
         <v>1.2474116208866605E-4</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <f>'Summary Qty'!A91</f>
         <v>613</v>
@@ -4324,7 +4324,7 @@
         <v>6.7360227527879669E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <f>'Summary Qty'!A92</f>
         <v>627</v>
@@ -4361,7 +4361,7 @@
         <v>4.9148017862934426E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <f>'Summary Qty'!A93</f>
         <v>642</v>
@@ -4398,7 +4398,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <f>'Summary Qty'!A94</f>
         <v>643</v>
@@ -4435,7 +4435,7 @@
         <v>4.241199511014646E-4</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <f>'Summary Qty'!A95</f>
         <v>651</v>
@@ -4472,7 +4472,7 @@
         <v>1.2474116208866605E-4</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <f>'Summary Qty'!A96</f>
         <v>652</v>
@@ -4509,7 +4509,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <f>'Summary Qty'!A97</f>
         <v>655</v>
@@ -4546,7 +4546,7 @@
         <v>2.7443055659506533E-4</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <f>'Summary Qty'!A98</f>
         <v>711</v>
@@ -4583,7 +4583,7 @@
         <v>3.4927525384826496E-4</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <f>'Summary Qty'!A99</f>
         <v>712</v>
@@ -4620,7 +4620,7 @@
         <v>1.4968939450639928E-4</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <f>'Summary Qty'!A100</f>
         <v>721</v>
@@ -4657,7 +4657,7 @@
         <v>2.2453409175959892E-4</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <f>'Summary Qty'!A101</f>
         <v>722</v>
@@ -4694,7 +4694,7 @@
         <v>7.4844697253199639E-5</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <f>'Summary Qty'!A102</f>
         <v>727</v>
@@ -4731,7 +4731,7 @@
         <v>1.2474116208866605E-4</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <f>'Summary Qty'!A103</f>
         <v>728</v>
@@ -4768,7 +4768,7 @@
         <v>1.2474116208866605E-4</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <f>'Summary Qty'!A104</f>
         <v>731</v>
@@ -4805,7 +4805,7 @@
         <v>7.2349874011426321E-4</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <f>'Summary Qty'!A105</f>
         <v>732</v>
@@ -4842,7 +4842,7 @@
         <v>2.2453409175959892E-4</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <f>'Summary Qty'!A106</f>
         <v>733</v>
@@ -4879,7 +4879,7 @@
         <v>1.5717386423171923E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <f>'Summary Qty'!A107</f>
         <v>736</v>
@@ -4916,7 +4916,7 @@
         <v>7.9834343736746275E-4</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <f>'Summary Qty'!A108</f>
         <v>741</v>
@@ -4953,7 +4953,7 @@
         <v>9.9792929670932843E-5</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <f>'Summary Qty'!A109</f>
         <v>743</v>
@@ -4990,7 +4990,7 @@
         <v>2.4948232417733209E-4</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <f>'Summary Qty'!A110</f>
         <v>744</v>
@@ -5027,7 +5027,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <f>'Summary Qty'!A111</f>
         <v>811</v>
@@ -5064,7 +5064,7 @@
         <v>2.7193573335329204E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <f>'Summary Qty'!A112</f>
         <v>825</v>
@@ -5101,7 +5101,7 @@
         <v>2.9688396577102522E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <f>'Summary Qty'!A113</f>
         <v>833</v>
@@ -5138,7 +5138,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <f>'Summary Qty'!A114</f>
         <v>845</v>
@@ -5175,7 +5175,7 @@
         <v>3.742234862659982E-4</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <f>'Summary Qty'!A115</f>
         <v>846</v>
@@ -5212,7 +5212,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <f>'Summary Qty'!A116</f>
         <v>872</v>
@@ -5249,7 +5249,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <f>'Summary Qty'!A117</f>
         <v>874</v>
@@ -5286,7 +5286,7 @@
         <v>2.2453409175959892E-4</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <f>'Summary Qty'!A118</f>
         <v>88943</v>
@@ -5323,7 +5323,7 @@
         <v>1.2224633884689274E-3</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <f>'Summary Qty'!A119</f>
         <v>915</v>
@@ -5360,7 +5360,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <f>'Summary Qty'!A120</f>
         <v>916</v>
@@ -5397,7 +5397,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <f>'Summary Qty'!A121</f>
         <v>926</v>
@@ -5434,7 +5434,7 @@
         <v>4.9896464835466423E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <f>'Summary Qty'!A122</f>
         <v>927</v>
@@ -5471,7 +5471,7 @@
         <v>1.0104034129181951E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <f>'Summary Qty'!A123</f>
         <v>943</v>
@@ -5508,7 +5508,7 @@
         <v>2.8440984956215861E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <f>'Summary Qty'!A124</f>
         <v>945</v>
@@ -5545,7 +5545,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <f>'Summary Qty'!A125</f>
         <v>949</v>
@@ -5582,7 +5582,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <f>'Summary Qty'!A126</f>
         <v>965</v>
@@ -5619,7 +5619,7 @@
         <v>1.7713245016590582E-3</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <f>'Summary Qty'!A127</f>
         <v>0</v>
@@ -5656,7 +5656,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <f>'Summary Qty'!A128</f>
         <v>981</v>
@@ -5693,7 +5693,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <f>'Summary Qty'!A129</f>
         <v>990</v>
@@ -5730,7 +5730,7 @@
         <v>5.4886111319013065E-4</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <f>'Summary Qty'!A130</f>
         <v>9999</v>
@@ -5767,7 +5767,7 @@
         <v>2.2079185689693893E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="str">
         <f>'Summary Qty'!A131</f>
         <v>Cem</v>
@@ -5804,7 +5804,7 @@
         <v>3.8669760247486478E-3</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="str">
         <f>'Summary Qty'!A132</f>
         <v>D9986</v>
@@ -5841,7 +5841,7 @@
         <v>3.1833944565027576E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="str">
         <f>'Summary Qty'!A133</f>
         <v>Insert</v>
@@ -5878,7 +5878,7 @@
         <v>3.4927525384826496E-4</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="str">
         <f>'Summary Qty'!A134</f>
         <v>Zclin</v>
@@ -5915,7 +5915,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <f>'Summary Qty'!A135</f>
         <v>15</v>
@@ -5952,7 +5952,7 @@
         <v>1.4968939450639928E-4</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <f>'Summary Qty'!A136</f>
         <v>19</v>
@@ -5989,7 +5989,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <f>'Summary Qty'!A137</f>
         <v>316</v>
@@ -6026,7 +6026,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <f>'Summary Qty'!A138</f>
         <v>165</v>
@@ -6063,7 +6063,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <f>'Summary Qty'!A139</f>
         <v>88322</v>
@@ -6100,7 +6100,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <f>'Summary Qty'!A140</f>
         <v>556</v>
@@ -6137,7 +6137,7 @@
         <v>5.4886111319013065E-4</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <f>'Summary Qty'!A141</f>
         <v>631</v>
@@ -6174,7 +6174,7 @@
         <v>9.9792929670932843E-5</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <f>'Summary Qty'!A142</f>
         <v>656</v>
@@ -6211,7 +6211,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <f>'Summary Qty'!A143</f>
         <v>753</v>
@@ -6248,7 +6248,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <f>'Summary Qty'!A144</f>
         <v>768</v>
@@ -6285,7 +6285,7 @@
         <v>2.2453409175959892E-4</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <f>'Summary Qty'!A145</f>
         <v>776</v>
@@ -6322,7 +6322,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <f>'Summary Qty'!A146</f>
         <v>823</v>
@@ -6359,7 +6359,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <f>'Summary Qty'!A147</f>
         <v>841</v>
@@ -6396,7 +6396,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <f>'Summary Qty'!A148</f>
         <v>873</v>
@@ -6433,7 +6433,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <f>'Summary Qty'!A149</f>
         <v>966</v>
@@ -6470,7 +6470,7 @@
         <v>1.2474116208866605E-4</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="str">
         <f>'Summary Qty'!A150</f>
         <v>Script</v>
@@ -6507,7 +6507,7 @@
         <v>2.2453409175959892E-4</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="str">
         <f>'Summary Qty'!A151</f>
         <v>CrownCem</v>
@@ -6544,7 +6544,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="str">
         <f>'Summary Qty'!A152</f>
         <v>Rev</v>
@@ -6581,7 +6581,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="str">
         <f>'Summary Qty'!A153</f>
         <v>Spl Ins</v>
@@ -6618,7 +6618,7 @@
         <v>7.4844697253199639E-5</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <f>'Summary Qty'!A154</f>
         <v>18</v>
@@ -6655,7 +6655,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="str">
         <f>'Summary Qty'!A155</f>
         <v>Add LA</v>
@@ -6692,7 +6692,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="str">
         <f>'Summary Qty'!A156</f>
         <v>InvisR</v>
@@ -6729,7 +6729,7 @@
         <v>2.4948232417733209E-4</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <f>'Summary Qty'!A157</f>
         <v>245</v>
@@ -6766,7 +6766,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <f>'Summary Qty'!A158</f>
         <v>451</v>
@@ -6803,7 +6803,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <f>'Summary Qty'!A159</f>
         <v>88535</v>
@@ -6840,7 +6840,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <f>'Summary Qty'!A160</f>
         <v>632</v>
@@ -6877,7 +6877,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <f>'Summary Qty'!A161</f>
         <v>658</v>
@@ -6914,7 +6914,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <f>'Summary Qty'!A162</f>
         <v>88522</v>
@@ -6951,7 +6951,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="str">
         <f>'Summary Qty'!A163</f>
         <v>Dr Invis Cons</v>
@@ -6988,7 +6988,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="str">
         <f>'Summary Qty'!A164</f>
         <v>FIC</v>
@@ -7025,7 +7025,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <f>'Summary Qty'!A165</f>
         <v>281</v>
@@ -7062,7 +7062,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <f>'Summary Qty'!A166</f>
         <v>618</v>
@@ -7127,7 +7127,7 @@
     <col min="15" max="15" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -7168,7 +7168,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>11</v>
       </c>
@@ -7212,7 +7212,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>12</v>
       </c>
@@ -7256,7 +7256,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>13</v>
       </c>
@@ -7300,7 +7300,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>14</v>
       </c>
@@ -7344,7 +7344,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>22</v>
       </c>
@@ -7388,7 +7388,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>24</v>
       </c>
@@ -7432,7 +7432,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>37</v>
       </c>
@@ -7476,7 +7476,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>61</v>
       </c>
@@ -7520,7 +7520,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>71</v>
       </c>
@@ -7564,7 +7564,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>72</v>
       </c>
@@ -7608,7 +7608,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>73</v>
       </c>
@@ -7652,7 +7652,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>74</v>
       </c>
@@ -7696,7 +7696,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>82</v>
       </c>
@@ -7740,7 +7740,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>88011</v>
       </c>
@@ -7784,7 +7784,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>88012</v>
       </c>
@@ -7828,7 +7828,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>88013</v>
       </c>
@@ -7872,7 +7872,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>88022</v>
       </c>
@@ -7916,7 +7916,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>18</v>
       </c>
@@ -7960,7 +7960,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>111</v>
       </c>
@@ -8004,7 +8004,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>113</v>
       </c>
@@ -8048,7 +8048,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>114</v>
       </c>
@@ -8092,7 +8092,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>115</v>
       </c>
@@ -8136,7 +8136,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>116</v>
       </c>
@@ -8180,7 +8180,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>117</v>
       </c>
@@ -8224,7 +8224,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>118</v>
       </c>
@@ -8268,7 +8268,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>119</v>
       </c>
@@ -8312,7 +8312,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>121</v>
       </c>
@@ -8356,7 +8356,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>123</v>
       </c>
@@ -8400,7 +8400,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>141</v>
       </c>
@@ -8444,7 +8444,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>151</v>
       </c>
@@ -8488,7 +8488,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>161</v>
       </c>
@@ -8532,7 +8532,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>171</v>
       </c>
@@ -8576,7 +8576,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>88111</v>
       </c>
@@ -8620,7 +8620,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>88114</v>
       </c>
@@ -8664,7 +8664,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>88115</v>
       </c>
@@ -8708,7 +8708,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>88121</v>
       </c>
@@ -8752,7 +8752,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>88161</v>
       </c>
@@ -8796,7 +8796,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>88162</v>
       </c>
@@ -8840,7 +8840,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>213</v>
       </c>
@@ -8884,7 +8884,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>221</v>
       </c>
@@ -8928,7 +8928,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>222</v>
       </c>
@@ -8972,7 +8972,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>231</v>
       </c>
@@ -9016,7 +9016,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>250</v>
       </c>
@@ -9060,7 +9060,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>251</v>
       </c>
@@ -9104,7 +9104,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>311</v>
       </c>
@@ -9148,7 +9148,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>314</v>
       </c>
@@ -9192,7 +9192,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>322</v>
       </c>
@@ -9236,7 +9236,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>323</v>
       </c>
@@ -9280,7 +9280,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>324</v>
       </c>
@@ -9324,7 +9324,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>391</v>
       </c>
@@ -9368,7 +9368,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>88311</v>
       </c>
@@ -9412,7 +9412,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>88314</v>
       </c>
@@ -9456,7 +9456,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>88316</v>
       </c>
@@ -9500,7 +9500,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>88324</v>
       </c>
@@ -9544,7 +9544,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>411</v>
       </c>
@@ -9588,7 +9588,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>414</v>
       </c>
@@ -9632,7 +9632,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>415</v>
       </c>
@@ -9676,7 +9676,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>416</v>
       </c>
@@ -9720,7 +9720,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>417</v>
       </c>
@@ -9764,7 +9764,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>418</v>
       </c>
@@ -9808,7 +9808,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>419</v>
       </c>
@@ -9852,7 +9852,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>431</v>
       </c>
@@ -9896,7 +9896,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>455</v>
       </c>
@@ -9940,7 +9940,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>88414</v>
       </c>
@@ -9984,7 +9984,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>521</v>
       </c>
@@ -10028,7 +10028,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>522</v>
       </c>
@@ -10072,7 +10072,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>523</v>
       </c>
@@ -10116,7 +10116,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>524</v>
       </c>
@@ -10160,7 +10160,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>525</v>
       </c>
@@ -10204,7 +10204,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>526</v>
       </c>
@@ -10248,7 +10248,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>531</v>
       </c>
@@ -10292,7 +10292,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>532</v>
       </c>
@@ -10336,7 +10336,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>533</v>
       </c>
@@ -10380,7 +10380,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>534</v>
       </c>
@@ -10424,7 +10424,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>535</v>
       </c>
@@ -10468,7 +10468,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>572</v>
       </c>
@@ -10512,7 +10512,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>574</v>
       </c>
@@ -10556,7 +10556,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>576</v>
       </c>
@@ -10600,7 +10600,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>577</v>
       </c>
@@ -10644,7 +10644,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>578</v>
       </c>
@@ -10688,7 +10688,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>88521</v>
       </c>
@@ -10732,7 +10732,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>88523</v>
       </c>
@@ -10776,7 +10776,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>88524</v>
       </c>
@@ -10820,7 +10820,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>88525</v>
       </c>
@@ -10864,7 +10864,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>88531</v>
       </c>
@@ -10908,7 +10908,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>88532</v>
       </c>
@@ -10952,7 +10952,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>88533</v>
       </c>
@@ -10996,7 +10996,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>88534</v>
       </c>
@@ -11040,7 +11040,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>88586</v>
       </c>
@@ -11084,7 +11084,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>613</v>
       </c>
@@ -11128,7 +11128,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>627</v>
       </c>
@@ -11172,7 +11172,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>642</v>
       </c>
@@ -11216,7 +11216,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>643</v>
       </c>
@@ -11260,7 +11260,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>651</v>
       </c>
@@ -11304,7 +11304,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>652</v>
       </c>
@@ -11348,7 +11348,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>655</v>
       </c>
@@ -11392,7 +11392,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>711</v>
       </c>
@@ -11436,7 +11436,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>712</v>
       </c>
@@ -11480,7 +11480,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>721</v>
       </c>
@@ -11524,7 +11524,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>722</v>
       </c>
@@ -11568,7 +11568,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>727</v>
       </c>
@@ -11612,7 +11612,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>728</v>
       </c>
@@ -11656,7 +11656,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>731</v>
       </c>
@@ -11700,7 +11700,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>732</v>
       </c>
@@ -11744,7 +11744,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>733</v>
       </c>
@@ -11788,7 +11788,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>736</v>
       </c>
@@ -11832,7 +11832,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>741</v>
       </c>
@@ -11876,7 +11876,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>743</v>
       </c>
@@ -11920,7 +11920,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>744</v>
       </c>
@@ -11964,7 +11964,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>811</v>
       </c>
@@ -12008,7 +12008,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>825</v>
       </c>
@@ -12052,7 +12052,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>833</v>
       </c>
@@ -12096,7 +12096,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>845</v>
       </c>
@@ -12140,7 +12140,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>846</v>
       </c>
@@ -12184,7 +12184,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>872</v>
       </c>
@@ -12228,7 +12228,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <v>874</v>
       </c>
@@ -12272,7 +12272,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>88943</v>
       </c>
@@ -12316,7 +12316,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>915</v>
       </c>
@@ -12360,7 +12360,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>916</v>
       </c>
@@ -12404,7 +12404,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <v>926</v>
       </c>
@@ -12448,7 +12448,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>927</v>
       </c>
@@ -12492,7 +12492,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <v>943</v>
       </c>
@@ -12536,7 +12536,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
         <v>945</v>
       </c>
@@ -12580,7 +12580,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <v>949</v>
       </c>
@@ -12624,7 +12624,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
         <v>965</v>
       </c>
@@ -12668,7 +12668,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A127" s="4">
         <v>0</v>
       </c>
@@ -12712,7 +12712,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
         <v>981</v>
       </c>
@@ -12756,7 +12756,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
         <v>990</v>
       </c>
@@ -12800,7 +12800,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A130" s="4">
         <v>9999</v>
       </c>
@@ -12844,7 +12844,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>19</v>
       </c>
@@ -12888,7 +12888,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
         <v>20</v>
       </c>
@@ -12932,7 +12932,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
         <v>21</v>
       </c>
@@ -12976,7 +12976,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
         <v>22</v>
       </c>
@@ -13020,7 +13020,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A135" s="4">
         <v>15</v>
       </c>
@@ -13064,7 +13064,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A136" s="4">
         <v>19</v>
       </c>
@@ -13108,7 +13108,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
         <v>316</v>
       </c>
@@ -13152,7 +13152,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A138" s="4">
         <v>165</v>
       </c>
@@ -13196,7 +13196,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A139" s="4">
         <v>88322</v>
       </c>
@@ -13240,7 +13240,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A140" s="4">
         <v>556</v>
       </c>
@@ -13284,7 +13284,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A141" s="4">
         <v>631</v>
       </c>
@@ -13328,7 +13328,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A142" s="4">
         <v>656</v>
       </c>
@@ -13372,7 +13372,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A143" s="4">
         <v>753</v>
       </c>
@@ -13416,7 +13416,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A144" s="4">
         <v>768</v>
       </c>
@@ -13460,7 +13460,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A145" s="4">
         <v>776</v>
       </c>
@@ -13504,7 +13504,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A146" s="4">
         <v>823</v>
       </c>
@@ -13548,7 +13548,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A147" s="4">
         <v>841</v>
       </c>
@@ -13592,7 +13592,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A148" s="4">
         <v>873</v>
       </c>
@@ -13636,7 +13636,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
         <v>966</v>
       </c>
@@ -13680,7 +13680,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A150" s="6" t="s">
         <v>23</v>
       </c>
@@ -13724,7 +13724,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A151" s="6" t="s">
         <v>24</v>
       </c>
@@ -13768,7 +13768,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A152" s="6" t="s">
         <v>25</v>
       </c>
@@ -13812,7 +13812,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A153" s="6" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Update Input_Preprocess for preprocessing 2
</commit_message>
<xml_diff>
--- a/Data/Real/DES - Clarity Dental.xlsx
+++ b/Data/Real/DES - Clarity Dental.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\radika\AI_Engineer\Project\Dental_Clinic\Code\Data\Real\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079B172E-5D32-4D8E-9C21-2614E0331387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5375C2-A23C-43F0-98E2-EC70147C47D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model_Input" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1321" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1322" uniqueCount="196">
   <si>
     <t>Category</t>
   </si>
@@ -631,7 +631,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -661,6 +661,20 @@
       <color theme="1"/>
       <name val="Aptos narrow"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -670,7 +684,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -678,11 +692,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -700,6 +729,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -920,8 +957,8 @@
   </sheetPr>
   <dimension ref="A1:R167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="A127" sqref="A127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -937,10 +974,9 @@
     <col min="14" max="14" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="str">
-        <f>'Summary Qty'!A1</f>
-        <v>Code</v>
+    <row r="1" spans="1:18" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -967,7 +1003,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <f>'Summary Qty'!A2</f>
         <v>11</v>
@@ -984,9 +1020,8 @@
         <f>'Summary Qty'!N2</f>
         <v>64.682493540051681</v>
       </c>
-      <c r="E2" s="1">
-        <f>'Summary Qty'!O2</f>
-        <v>45</v>
+      <c r="E2" s="11">
+        <v>30</v>
       </c>
       <c r="F2" s="1">
         <f t="shared" ref="F2:F166" si="0">D2*60%</f>
@@ -1004,7 +1039,7 @@
         <v>3.8619863782651011E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>'Summary Qty'!A3</f>
         <v>12</v>
@@ -1021,9 +1056,8 @@
         <f>'Summary Qty'!N3</f>
         <v>60.530227471566057</v>
       </c>
-      <c r="E3" s="1">
-        <f>'Summary Qty'!O3</f>
-        <v>44</v>
+      <c r="E3" s="11">
+        <v>15</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" si="0"/>
@@ -1041,7 +1075,7 @@
         <v>5.7031659306938126E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f>'Summary Qty'!A4</f>
         <v>13</v>
@@ -1058,9 +1092,8 @@
         <f>'Summary Qty'!N4</f>
         <v>51.481676190476186</v>
       </c>
-      <c r="E4" s="1">
-        <f>'Summary Qty'!O4</f>
-        <v>30</v>
+      <c r="E4" s="11">
+        <v>15</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
@@ -1078,7 +1111,7 @@
         <v>2.6195644038619875E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f>'Summary Qty'!A5</f>
         <v>14</v>
@@ -1095,9 +1128,8 @@
         <f>'Summary Qty'!N5</f>
         <v>70.080152671755727</v>
       </c>
-      <c r="E5" s="1">
-        <f>'Summary Qty'!O5</f>
-        <v>30</v>
+      <c r="E5" s="11">
+        <v>15</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
@@ -1121,7 +1153,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f>'Summary Qty'!A6</f>
         <v>22</v>
@@ -1138,9 +1170,8 @@
         <f>'Summary Qty'!N6</f>
         <v>48.085593162000919</v>
       </c>
-      <c r="E6" s="1">
-        <f>'Summary Qty'!O6</f>
-        <v>44</v>
+      <c r="E6" s="11">
+        <v>15</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
@@ -1167,7 +1198,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f>'Summary Qty'!A7</f>
         <v>24</v>
@@ -1184,9 +1215,8 @@
         <f>'Summary Qty'!N7</f>
         <v>28.552580645161289</v>
       </c>
-      <c r="E7" s="1">
-        <f>'Summary Qty'!O7</f>
-        <v>45</v>
+      <c r="E7" s="11">
+        <v>17.37</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
@@ -1210,7 +1240,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f>'Summary Qty'!A8</f>
         <v>37</v>
@@ -1227,9 +1257,8 @@
         <f>'Summary Qty'!N8</f>
         <v>91.709758771929813</v>
       </c>
-      <c r="E8" s="1">
-        <f>'Summary Qty'!O8</f>
-        <v>23</v>
+      <c r="E8" s="11">
+        <v>15</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
@@ -1250,7 +1279,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f>'Summary Qty'!A9</f>
         <v>61</v>
@@ -1267,9 +1296,8 @@
         <f>'Summary Qty'!N9</f>
         <v>20.676923076923078</v>
       </c>
-      <c r="E9" s="1">
-        <f>'Summary Qty'!O9</f>
-        <v>33</v>
+      <c r="E9" s="11">
+        <v>10</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
@@ -1287,7 +1315,7 @@
         <v>9.7298106429159531E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f>'Summary Qty'!A10</f>
         <v>71</v>
@@ -1304,9 +1332,8 @@
         <f>'Summary Qty'!N10</f>
         <v>74.286571428571435</v>
       </c>
-      <c r="E10" s="1">
-        <f>'Summary Qty'!O10</f>
-        <v>19</v>
+      <c r="E10" s="11">
+        <v>30</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="0"/>
@@ -1324,7 +1351,7 @@
         <v>1.7463762692413248E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f>'Summary Qty'!A11</f>
         <v>72</v>
@@ -1341,9 +1368,8 @@
         <f>'Summary Qty'!N11</f>
         <v>41.506476683937827</v>
       </c>
-      <c r="E11" s="1">
-        <f>'Summary Qty'!O11</f>
-        <v>57</v>
+      <c r="E11" s="11">
+        <v>10</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="0"/>
@@ -1361,7 +1387,7 @@
         <v>2.8890053139735056E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f>'Summary Qty'!A12</f>
         <v>73</v>
@@ -1378,9 +1404,8 @@
         <f>'Summary Qty'!N12</f>
         <v>47.663636363636371</v>
       </c>
-      <c r="E12" s="1">
-        <f>'Summary Qty'!O12</f>
-        <v>37</v>
+      <c r="E12" s="11">
+        <v>10</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="0"/>
@@ -1398,7 +1423,7 @@
         <v>5.4886111319013065E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f>'Summary Qty'!A13</f>
         <v>74</v>
@@ -1415,9 +1440,8 @@
         <f>'Summary Qty'!N13</f>
         <v>212.08</v>
       </c>
-      <c r="E13" s="1">
-        <f>'Summary Qty'!O13</f>
-        <v>39</v>
+      <c r="E13" s="11">
+        <v>15</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="0"/>
@@ -1438,7 +1462,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f>'Summary Qty'!A14</f>
         <v>82</v>
@@ -1455,9 +1479,8 @@
         <f>'Summary Qty'!N14</f>
         <v>85</v>
       </c>
-      <c r="E14" s="1">
-        <f>'Summary Qty'!O14</f>
-        <v>26</v>
+      <c r="E14" s="11">
+        <v>15</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
@@ -1475,7 +1498,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f>'Summary Qty'!A15</f>
         <v>88011</v>
@@ -1492,9 +1515,8 @@
         <f>'Summary Qty'!N15</f>
         <v>53.57990353697749</v>
       </c>
-      <c r="E15" s="1">
-        <f>'Summary Qty'!O15</f>
-        <v>17</v>
+      <c r="E15" s="11">
+        <v>30</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="0"/>
@@ -1512,7 +1534,7 @@
         <v>7.7589002819150286E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f>'Summary Qty'!A16</f>
         <v>88012</v>
@@ -1529,9 +1551,8 @@
         <f>'Summary Qty'!N16</f>
         <v>44.610628742514969</v>
       </c>
-      <c r="E16" s="1">
-        <f>'Summary Qty'!O16</f>
-        <v>37</v>
+      <c r="E16" s="11">
+        <v>15</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="0"/>
@@ -1549,7 +1570,7 @@
         <v>8.3327096275228937E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f>'Summary Qty'!A17</f>
         <v>88013</v>
@@ -1566,9 +1587,8 @@
         <f>'Summary Qty'!N17</f>
         <v>28.001886792452829</v>
       </c>
-      <c r="E17" s="1">
-        <f>'Summary Qty'!O17</f>
-        <v>42</v>
+      <c r="E17" s="11">
+        <v>15</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="0"/>
@@ -1586,7 +1606,7 @@
         <v>2.6445126362797207E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <f>'Summary Qty'!A18</f>
         <v>88022</v>
@@ -1603,9 +1623,8 @@
         <f>'Summary Qty'!N18</f>
         <v>30.964991181657851</v>
       </c>
-      <c r="E18" s="1">
-        <f>'Summary Qty'!O18</f>
-        <v>58</v>
+      <c r="E18" s="11">
+        <v>15</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="0"/>
@@ -1623,7 +1642,7 @@
         <v>1.4145647780854731E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="str">
         <f>'Summary Qty'!A19</f>
         <v>CC</v>
@@ -1640,9 +1659,8 @@
         <f>'Summary Qty'!N19</f>
         <v>60</v>
       </c>
-      <c r="E19" s="1">
-        <f>'Summary Qty'!O19</f>
-        <v>57</v>
+      <c r="E19" s="11">
+        <v>17.37</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="0"/>
@@ -1660,7 +1678,7 @@
         <v>7.4844697253199639E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f>'Summary Qty'!A20</f>
         <v>111</v>
@@ -1677,9 +1695,8 @@
         <f>'Summary Qty'!N20</f>
         <v>60</v>
       </c>
-      <c r="E20" s="1">
-        <f>'Summary Qty'!O20</f>
-        <v>54</v>
+      <c r="E20" s="11">
+        <v>15</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="0"/>
@@ -1697,7 +1714,7 @@
         <v>1.4968939450639928E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f>'Summary Qty'!A21</f>
         <v>113</v>
@@ -1714,9 +1731,8 @@
         <f>'Summary Qty'!N21</f>
         <v>18.464143426294822</v>
       </c>
-      <c r="E21" s="1">
-        <f>'Summary Qty'!O21</f>
-        <v>49</v>
+      <c r="E21" s="11">
+        <v>15</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="0"/>
@@ -1734,7 +1750,7 @@
         <v>6.2620063368510363E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f>'Summary Qty'!A22</f>
         <v>114</v>
@@ -1751,9 +1767,8 @@
         <f>'Summary Qty'!N22</f>
         <v>127.17393302371059</v>
       </c>
-      <c r="E22" s="1">
-        <f>'Summary Qty'!O22</f>
-        <v>22</v>
+      <c r="E22" s="11">
+        <v>40</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="0"/>
@@ -1771,7 +1786,7 @@
         <v>0.10206321882094657</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f>'Summary Qty'!A23</f>
         <v>115</v>
@@ -1788,9 +1803,8 @@
         <f>'Summary Qty'!N23</f>
         <v>122.67185185185186</v>
       </c>
-      <c r="E23" s="1">
-        <f>'Summary Qty'!O23</f>
-        <v>50</v>
+      <c r="E23" s="11">
+        <v>20</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="0"/>
@@ -1808,7 +1822,7 @@
         <v>3.3680113763939834E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f>'Summary Qty'!A24</f>
         <v>116</v>
@@ -1825,9 +1839,8 @@
         <f>'Summary Qty'!N24</f>
         <v>78</v>
       </c>
-      <c r="E24" s="1">
-        <f>'Summary Qty'!O24</f>
-        <v>58</v>
+      <c r="E24" s="11">
+        <v>10</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="0"/>
@@ -1845,7 +1858,7 @@
         <v>7.4844697253199639E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f>'Summary Qty'!A25</f>
         <v>117</v>
@@ -1862,9 +1875,8 @@
         <f>'Summary Qty'!N25</f>
         <v>256</v>
       </c>
-      <c r="E25" s="1">
-        <f>'Summary Qty'!O25</f>
-        <v>41</v>
+      <c r="E25" s="11">
+        <v>15</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" si="0"/>
@@ -1882,7 +1894,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f>'Summary Qty'!A26</f>
         <v>118</v>
@@ -1899,9 +1911,8 @@
         <f>'Summary Qty'!N26</f>
         <v>65.662279511533256</v>
       </c>
-      <c r="E26" s="1">
-        <f>'Summary Qty'!O26</f>
-        <v>57</v>
+      <c r="E26" s="11">
+        <v>3</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" si="0"/>
@@ -1919,7 +1930,7 @@
         <v>1.8386847291869377E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f>'Summary Qty'!A27</f>
         <v>119</v>
@@ -1936,9 +1947,8 @@
         <f>'Summary Qty'!N27</f>
         <v>102.76644736842107</v>
       </c>
-      <c r="E27" s="1">
-        <f>'Summary Qty'!O27</f>
-        <v>47</v>
+      <c r="E27" s="11">
+        <v>15</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" si="0"/>
@@ -1956,7 +1966,7 @@
         <v>5.6881969912431721E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f>'Summary Qty'!A28</f>
         <v>121</v>
@@ -1973,9 +1983,8 @@
         <f>'Summary Qty'!N28</f>
         <v>41.126063168366073</v>
       </c>
-      <c r="E28" s="1">
-        <f>'Summary Qty'!O28</f>
-        <v>46</v>
+      <c r="E28" s="11">
+        <v>30</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" si="0"/>
@@ -1993,7 +2002,7 @@
         <v>0.10031684255170524</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f>'Summary Qty'!A29</f>
         <v>123</v>
@@ -2010,9 +2019,8 @@
         <f>'Summary Qty'!N29</f>
         <v>35.055555555555557</v>
       </c>
-      <c r="E29" s="1">
-        <f>'Summary Qty'!O29</f>
-        <v>59</v>
+      <c r="E29" s="11">
+        <v>10</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" si="0"/>
@@ -2030,7 +2038,7 @@
         <v>4.4906818351919784E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f>'Summary Qty'!A30</f>
         <v>141</v>
@@ -2047,9 +2055,8 @@
         <f>'Summary Qty'!N30</f>
         <v>52.462500000000006</v>
       </c>
-      <c r="E30" s="1">
-        <f>'Summary Qty'!O30</f>
-        <v>28</v>
+      <c r="E30" s="11">
+        <v>15</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" si="0"/>
@@ -2067,7 +2074,7 @@
         <v>9.9792929670932843E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <f>'Summary Qty'!A31</f>
         <v>151</v>
@@ -2084,9 +2091,8 @@
         <f>'Summary Qty'!N31</f>
         <v>189.44117647058823</v>
       </c>
-      <c r="E31" s="1">
-        <f>'Summary Qty'!O31</f>
-        <v>50</v>
+      <c r="E31" s="11">
+        <v>15</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" si="0"/>
@@ -2104,7 +2110,7 @@
         <v>8.4823990220292921E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <f>'Summary Qty'!A32</f>
         <v>161</v>
@@ -2121,9 +2127,8 @@
         <f>'Summary Qty'!N32</f>
         <v>61.674786324786325</v>
       </c>
-      <c r="E32" s="1">
-        <f>'Summary Qty'!O32</f>
-        <v>44</v>
+      <c r="E32" s="11">
+        <v>15</v>
       </c>
       <c r="F32" s="1">
         <f t="shared" si="0"/>
@@ -2141,7 +2146,7 @@
         <v>2.9189431928747858E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <f>'Summary Qty'!A33</f>
         <v>171</v>
@@ -2158,9 +2163,8 @@
         <f>'Summary Qty'!N33</f>
         <v>21.252238805970151</v>
       </c>
-      <c r="E33" s="1">
-        <f>'Summary Qty'!O33</f>
-        <v>29</v>
+      <c r="E33" s="11">
+        <v>5</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" si="0"/>
@@ -2178,7 +2182,7 @@
         <v>1.671531571988125E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <f>'Summary Qty'!A34</f>
         <v>88111</v>
@@ -2195,9 +2199,8 @@
         <f>'Summary Qty'!N34</f>
         <v>54.966666666666669</v>
       </c>
-      <c r="E34" s="1">
-        <f>'Summary Qty'!O34</f>
-        <v>60</v>
+      <c r="E34" s="11">
+        <v>15</v>
       </c>
       <c r="F34" s="1">
         <f t="shared" si="0"/>
@@ -2215,7 +2218,7 @@
         <v>2.2453409175959892E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <f>'Summary Qty'!A35</f>
         <v>88114</v>
@@ -2232,9 +2235,8 @@
         <f>'Summary Qty'!N35</f>
         <v>91.333561643835608</v>
       </c>
-      <c r="E35" s="1">
-        <f>'Summary Qty'!O35</f>
-        <v>21</v>
+      <c r="E35" s="11">
+        <v>40</v>
       </c>
       <c r="F35" s="1">
         <f t="shared" si="0"/>
@@ -2252,7 +2254,7 @@
         <v>1.2748546765461671E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <f>'Summary Qty'!A36</f>
         <v>88115</v>
@@ -2269,9 +2271,8 @@
         <f>'Summary Qty'!N36</f>
         <v>59.662500000000001</v>
       </c>
-      <c r="E36" s="1">
-        <f>'Summary Qty'!O36</f>
-        <v>41</v>
+      <c r="E36" s="11">
+        <v>20</v>
       </c>
       <c r="F36" s="1">
         <f t="shared" si="0"/>
@@ -2289,7 +2290,7 @@
         <v>9.9792929670932843E-5</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <f>'Summary Qty'!A37</f>
         <v>88121</v>
@@ -2306,9 +2307,8 @@
         <f>'Summary Qty'!N37</f>
         <v>35.187406716417904</v>
       </c>
-      <c r="E37" s="1">
-        <f>'Summary Qty'!O37</f>
-        <v>50</v>
+      <c r="E37" s="11">
+        <v>30</v>
       </c>
       <c r="F37" s="1">
         <f t="shared" si="0"/>
@@ -2326,7 +2326,7 @@
         <v>1.3372252575905E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <f>'Summary Qty'!A38</f>
         <v>88161</v>
@@ -2343,9 +2343,8 @@
         <f>'Summary Qty'!N38</f>
         <v>46.851818181818189</v>
       </c>
-      <c r="E38" s="1">
-        <f>'Summary Qty'!O38</f>
-        <v>26</v>
+      <c r="E38" s="11">
+        <v>15</v>
       </c>
       <c r="F38" s="1">
         <f t="shared" si="0"/>
@@ -2363,7 +2362,7 @@
         <v>2.7443055659506534E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <f>'Summary Qty'!A39</f>
         <v>88162</v>
@@ -2380,9 +2379,8 @@
         <f>'Summary Qty'!N39</f>
         <v>23.396153846153844</v>
       </c>
-      <c r="E39" s="1">
-        <f>'Summary Qty'!O39</f>
-        <v>18</v>
+      <c r="E39" s="11">
+        <v>17.899999999999999</v>
       </c>
       <c r="F39" s="1">
         <f t="shared" si="0"/>
@@ -2400,7 +2398,7 @@
         <v>3.2432702143053173E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <f>'Summary Qty'!A40</f>
         <v>213</v>
@@ -2417,9 +2415,8 @@
         <f>'Summary Qty'!N40</f>
         <v>109.15166666666667</v>
       </c>
-      <c r="E40" s="1">
-        <f>'Summary Qty'!O40</f>
-        <v>34</v>
+      <c r="E40" s="11">
+        <v>30</v>
       </c>
       <c r="F40" s="1">
         <f t="shared" si="0"/>
@@ -2437,7 +2434,7 @@
         <v>4.4906818351919784E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <f>'Summary Qty'!A41</f>
         <v>221</v>
@@ -2454,9 +2451,8 @@
         <f>'Summary Qty'!N41</f>
         <v>54.765311004784692</v>
       </c>
-      <c r="E41" s="1">
-        <f>'Summary Qty'!O41</f>
-        <v>58</v>
+      <c r="E41" s="11">
+        <v>15</v>
       </c>
       <c r="F41" s="1">
         <f t="shared" si="0"/>
@@ -2474,7 +2470,7 @@
         <v>5.2141805753062416E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <f>'Summary Qty'!A42</f>
         <v>222</v>
@@ -2491,9 +2487,8 @@
         <f>'Summary Qty'!N42</f>
         <v>59.038304721030038</v>
       </c>
-      <c r="E42" s="1">
-        <f>'Summary Qty'!O42</f>
-        <v>24</v>
+      <c r="E42" s="11">
+        <v>5</v>
       </c>
       <c r="F42" s="1">
         <f t="shared" si="0"/>
@@ -2511,7 +2506,7 @@
         <v>1.1625876306663676E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <f>'Summary Qty'!A43</f>
         <v>231</v>
@@ -2528,9 +2523,8 @@
         <f>'Summary Qty'!N43</f>
         <v>88.05740740740741</v>
       </c>
-      <c r="E43" s="1">
-        <f>'Summary Qty'!O43</f>
-        <v>59</v>
+      <c r="E43" s="11">
+        <v>15</v>
       </c>
       <c r="F43" s="1">
         <f t="shared" si="0"/>
@@ -2548,7 +2542,7 @@
         <v>1.3472045505575933E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <f>'Summary Qty'!A44</f>
         <v>250</v>
@@ -2565,9 +2559,8 @@
         <f>'Summary Qty'!N44</f>
         <v>211.33168316831683</v>
       </c>
-      <c r="E44" s="1">
-        <f>'Summary Qty'!O44</f>
-        <v>30</v>
+      <c r="E44" s="12">
+        <v>60</v>
       </c>
       <c r="F44" s="1">
         <f t="shared" si="0"/>
@@ -2585,7 +2578,7 @@
         <v>5.0395429483821082E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <f>'Summary Qty'!A45</f>
         <v>251</v>
@@ -2602,9 +2595,8 @@
         <f>'Summary Qty'!N45</f>
         <v>265</v>
       </c>
-      <c r="E45" s="1">
-        <f>'Summary Qty'!O45</f>
-        <v>49</v>
+      <c r="E45" s="12">
+        <v>30</v>
       </c>
       <c r="F45" s="1">
         <f t="shared" si="0"/>
@@ -2622,7 +2614,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <f>'Summary Qty'!A46</f>
         <v>311</v>
@@ -2639,9 +2631,8 @@
         <f>'Summary Qty'!N46</f>
         <v>222.4725563063063</v>
       </c>
-      <c r="E46" s="1">
-        <f>'Summary Qty'!O46</f>
-        <v>56</v>
+      <c r="E46" s="12">
+        <v>30</v>
       </c>
       <c r="F46" s="1">
         <f t="shared" si="0"/>
@@ -2659,7 +2650,7 @@
         <v>2.2154030386947091E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <f>'Summary Qty'!A47</f>
         <v>314</v>
@@ -2676,9 +2667,8 @@
         <f>'Summary Qty'!N47</f>
         <v>257.15225806451616</v>
       </c>
-      <c r="E47" s="1">
-        <f>'Summary Qty'!O47</f>
-        <v>38</v>
+      <c r="E47" s="12">
+        <v>45</v>
       </c>
       <c r="F47" s="1">
         <f t="shared" si="0"/>
@@ -2696,7 +2686,7 @@
         <v>2.3201856148491887E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <f>'Summary Qty'!A48</f>
         <v>322</v>
@@ -2713,9 +2703,8 @@
         <f>'Summary Qty'!N48</f>
         <v>321.59499999999997</v>
       </c>
-      <c r="E48" s="1">
-        <f>'Summary Qty'!O48</f>
-        <v>27</v>
+      <c r="E48" s="11">
+        <v>45</v>
       </c>
       <c r="F48" s="1">
         <f t="shared" si="0"/>
@@ -2733,7 +2722,7 @@
         <v>1.1975151560511942E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <f>'Summary Qty'!A49</f>
         <v>323</v>
@@ -2750,9 +2739,8 @@
         <f>'Summary Qty'!N49</f>
         <v>401.77763157894736</v>
       </c>
-      <c r="E49" s="1">
-        <f>'Summary Qty'!O49</f>
-        <v>16</v>
+      <c r="E49" s="11">
+        <v>75</v>
       </c>
       <c r="F49" s="1">
         <f t="shared" si="0"/>
@@ -2770,7 +2758,7 @@
         <v>9.4803283187386202E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <f>'Summary Qty'!A50</f>
         <v>324</v>
@@ -2787,9 +2775,8 @@
         <f>'Summary Qty'!N50</f>
         <v>424.63841463414633</v>
       </c>
-      <c r="E50" s="1">
-        <f>'Summary Qty'!O50</f>
-        <v>43</v>
+      <c r="E50" s="11">
+        <v>100</v>
       </c>
       <c r="F50" s="1">
         <f t="shared" si="0"/>
@@ -2807,7 +2794,7 @@
         <v>2.0457550582541235E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <f>'Summary Qty'!A51</f>
         <v>391</v>
@@ -2824,9 +2811,8 @@
         <f>'Summary Qty'!N51</f>
         <v>455.66666666666669</v>
       </c>
-      <c r="E51" s="1">
-        <f>'Summary Qty'!O51</f>
-        <v>34</v>
+      <c r="E51" s="11">
+        <v>75</v>
       </c>
       <c r="F51" s="1">
         <f t="shared" si="0"/>
@@ -2844,7 +2830,7 @@
         <v>1.4968939450639928E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <f>'Summary Qty'!A52</f>
         <v>88311</v>
@@ -2861,9 +2847,8 @@
         <f>'Summary Qty'!N52</f>
         <v>133.6575</v>
       </c>
-      <c r="E52" s="1">
-        <f>'Summary Qty'!O52</f>
-        <v>18</v>
+      <c r="E52" s="12">
+        <v>30</v>
       </c>
       <c r="F52" s="1">
         <f t="shared" si="0"/>
@@ -2881,7 +2866,7 @@
         <v>9.9792929670932838E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <f>'Summary Qty'!A53</f>
         <v>88314</v>
@@ -2898,9 +2883,8 @@
         <f>'Summary Qty'!N53</f>
         <v>171.64999999999998</v>
       </c>
-      <c r="E53" s="1">
-        <f>'Summary Qty'!O53</f>
-        <v>49</v>
+      <c r="E53" s="12">
+        <v>45</v>
       </c>
       <c r="F53" s="1">
         <f t="shared" si="0"/>
@@ -2918,7 +2902,7 @@
         <v>9.9792929670932843E-5</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <f>'Summary Qty'!A54</f>
         <v>88316</v>
@@ -2935,9 +2919,8 @@
         <f>'Summary Qty'!N54</f>
         <v>84.603846153846149</v>
       </c>
-      <c r="E54" s="1">
-        <f>'Summary Qty'!O54</f>
-        <v>50</v>
+      <c r="E54" s="11">
+        <v>57.22</v>
       </c>
       <c r="F54" s="1">
         <f t="shared" si="0"/>
@@ -2955,7 +2938,7 @@
         <v>3.2432702143053173E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <f>'Summary Qty'!A55</f>
         <v>88324</v>
@@ -2972,9 +2955,8 @@
         <f>'Summary Qty'!N55</f>
         <v>327.35000000000002</v>
       </c>
-      <c r="E55" s="1">
-        <f>'Summary Qty'!O55</f>
-        <v>53</v>
+      <c r="E55" s="11">
+        <v>100</v>
       </c>
       <c r="F55" s="1">
         <f t="shared" si="0"/>
@@ -2992,7 +2974,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <f>'Summary Qty'!A56</f>
         <v>411</v>
@@ -3009,9 +2991,8 @@
         <f>'Summary Qty'!N56</f>
         <v>41.5</v>
       </c>
-      <c r="E56" s="1">
-        <f>'Summary Qty'!O56</f>
-        <v>32</v>
+      <c r="E56" s="12">
+        <v>30</v>
       </c>
       <c r="F56" s="1">
         <f t="shared" si="0"/>
@@ -3029,7 +3010,7 @@
         <v>2.9937878901279856E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <f>'Summary Qty'!A57</f>
         <v>414</v>
@@ -3046,9 +3027,8 @@
         <f>'Summary Qty'!N57</f>
         <v>75.650000000000006</v>
       </c>
-      <c r="E57" s="1">
-        <f>'Summary Qty'!O57</f>
-        <v>47</v>
+      <c r="E57" s="12">
+        <v>30</v>
       </c>
       <c r="F57" s="1">
         <f t="shared" si="0"/>
@@ -3066,7 +3046,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <f>'Summary Qty'!A58</f>
         <v>415</v>
@@ -3083,9 +3063,8 @@
         <f>'Summary Qty'!N58</f>
         <v>353.22750000000002</v>
       </c>
-      <c r="E58" s="1">
-        <f>'Summary Qty'!O58</f>
-        <v>57</v>
+      <c r="E58" s="12">
+        <v>15</v>
       </c>
       <c r="F58" s="1">
         <f t="shared" si="0"/>
@@ -3103,7 +3082,7 @@
         <v>1.4968939450639928E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <f>'Summary Qty'!A59</f>
         <v>416</v>
@@ -3120,9 +3099,8 @@
         <f>'Summary Qty'!N59</f>
         <v>160.79838709677421</v>
       </c>
-      <c r="E59" s="1">
-        <f>'Summary Qty'!O59</f>
-        <v>51</v>
+      <c r="E59" s="12">
+        <v>15</v>
       </c>
       <c r="F59" s="1">
         <f t="shared" si="0"/>
@@ -3140,7 +3118,7 @@
         <v>1.5467904098994591E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <f>'Summary Qty'!A60</f>
         <v>417</v>
@@ -3157,9 +3135,8 @@
         <f>'Summary Qty'!N60</f>
         <v>353.17542372881354</v>
       </c>
-      <c r="E60" s="1">
-        <f>'Summary Qty'!O60</f>
-        <v>51</v>
+      <c r="E60" s="12">
+        <v>15</v>
       </c>
       <c r="F60" s="1">
         <f t="shared" si="0"/>
@@ -3177,7 +3154,7 @@
         <v>1.4719457126462594E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <f>'Summary Qty'!A61</f>
         <v>418</v>
@@ -3194,9 +3171,8 @@
         <f>'Summary Qty'!N61</f>
         <v>153.68813559322035</v>
       </c>
-      <c r="E61" s="1">
-        <f>'Summary Qty'!O61</f>
-        <v>46</v>
+      <c r="E61" s="12">
+        <v>15</v>
       </c>
       <c r="F61" s="1">
         <f t="shared" si="0"/>
@@ -3214,7 +3190,7 @@
         <v>1.4719457126462594E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <f>'Summary Qty'!A62</f>
         <v>419</v>
@@ -3231,9 +3207,8 @@
         <f>'Summary Qty'!N62</f>
         <v>269.34256756756758</v>
       </c>
-      <c r="E62" s="1">
-        <f>'Summary Qty'!O62</f>
-        <v>27</v>
+      <c r="E62" s="12">
+        <v>15</v>
       </c>
       <c r="F62" s="1">
         <f t="shared" si="0"/>
@@ -3251,7 +3226,7 @@
         <v>1.8461691989122579E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <f>'Summary Qty'!A63</f>
         <v>431</v>
@@ -3268,9 +3243,8 @@
         <f>'Summary Qty'!N63</f>
         <v>100</v>
       </c>
-      <c r="E63" s="1">
-        <f>'Summary Qty'!O63</f>
-        <v>58</v>
+      <c r="E63" s="11">
+        <v>21</v>
       </c>
       <c r="F63" s="1">
         <f t="shared" si="0"/>
@@ -3288,7 +3262,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <f>'Summary Qty'!A64</f>
         <v>455</v>
@@ -3305,9 +3279,8 @@
         <f>'Summary Qty'!N64</f>
         <v>179.76666666666665</v>
       </c>
-      <c r="E64" s="1">
-        <f>'Summary Qty'!O64</f>
-        <v>19</v>
+      <c r="E64" s="12">
+        <v>15</v>
       </c>
       <c r="F64" s="1">
         <f t="shared" si="0"/>
@@ -3325,7 +3298,7 @@
         <v>4.4906818351919784E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <f>'Summary Qty'!A65</f>
         <v>88414</v>
@@ -3342,9 +3315,8 @@
         <f>'Summary Qty'!N65</f>
         <v>76.716666666666654</v>
       </c>
-      <c r="E65" s="1">
-        <f>'Summary Qty'!O65</f>
-        <v>19</v>
+      <c r="E65" s="12">
+        <v>30</v>
       </c>
       <c r="F65" s="1">
         <f t="shared" si="0"/>
@@ -3362,7 +3334,7 @@
         <v>7.4844697253199639E-5</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <f>'Summary Qty'!A66</f>
         <v>521</v>
@@ -3379,9 +3351,8 @@
         <f>'Summary Qty'!N66</f>
         <v>190.58470149253731</v>
       </c>
-      <c r="E66" s="1">
-        <f>'Summary Qty'!O66</f>
-        <v>34</v>
+      <c r="E66" s="12">
+        <v>15</v>
       </c>
       <c r="F66" s="1">
         <f t="shared" si="0"/>
@@ -3399,7 +3370,7 @@
         <v>3.34306314397625E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <f>'Summary Qty'!A67</f>
         <v>522</v>
@@ -3416,9 +3387,8 @@
         <f>'Summary Qty'!N67</f>
         <v>206.65867768595041</v>
       </c>
-      <c r="E67" s="1">
-        <f>'Summary Qty'!O67</f>
-        <v>30</v>
+      <c r="E67" s="12">
+        <v>25</v>
       </c>
       <c r="F67" s="1">
         <f t="shared" si="0"/>
@@ -3436,7 +3406,7 @@
         <v>3.0187361225457185E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <f>'Summary Qty'!A68</f>
         <v>523</v>
@@ -3453,9 +3423,8 @@
         <f>'Summary Qty'!N68</f>
         <v>231.39393162393162</v>
       </c>
-      <c r="E68" s="1">
-        <f>'Summary Qty'!O68</f>
-        <v>36</v>
+      <c r="E68" s="12">
+        <v>25</v>
       </c>
       <c r="F68" s="1">
         <f t="shared" si="0"/>
@@ -3473,7 +3442,7 @@
         <v>5.8378863857495716E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <f>'Summary Qty'!A69</f>
         <v>524</v>
@@ -3490,9 +3459,8 @@
         <f>'Summary Qty'!N69</f>
         <v>255.61247706422017</v>
       </c>
-      <c r="E69" s="1">
-        <f>'Summary Qty'!O69</f>
-        <v>20</v>
+      <c r="E69" s="12">
+        <v>25</v>
       </c>
       <c r="F69" s="1">
         <f t="shared" si="0"/>
@@ -3510,7 +3478,7 @@
         <v>5.4387146670658408E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <f>'Summary Qty'!A70</f>
         <v>525</v>
@@ -3527,9 +3495,8 @@
         <f>'Summary Qty'!N70</f>
         <v>318.73985401459856</v>
       </c>
-      <c r="E70" s="1">
-        <f>'Summary Qty'!O70</f>
-        <v>32</v>
+      <c r="E70" s="12">
+        <v>25</v>
       </c>
       <c r="F70" s="1">
         <f t="shared" si="0"/>
@@ -3547,7 +3514,7 @@
         <v>3.4179078412294498E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <f>'Summary Qty'!A71</f>
         <v>526</v>
@@ -3564,9 +3531,8 @@
         <f>'Summary Qty'!N71</f>
         <v>400.33333333333331</v>
       </c>
-      <c r="E71" s="1">
-        <f>'Summary Qty'!O71</f>
-        <v>60</v>
+      <c r="E71" s="11">
+        <v>31</v>
       </c>
       <c r="F71" s="1">
         <f t="shared" si="0"/>
@@ -3584,7 +3550,7 @@
         <v>6.7360227527879664E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <f>'Summary Qty'!A72</f>
         <v>531</v>
@@ -3601,9 +3567,8 @@
         <f>'Summary Qty'!N72</f>
         <v>185.7357650695518</v>
       </c>
-      <c r="E72" s="1">
-        <f>'Summary Qty'!O72</f>
-        <v>60</v>
+      <c r="E72" s="12">
+        <v>30</v>
       </c>
       <c r="F72" s="1">
         <f t="shared" si="0"/>
@@ -3621,7 +3586,7 @@
         <v>1.6141506374273386E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <f>'Summary Qty'!A73</f>
         <v>532</v>
@@ -3638,9 +3603,8 @@
         <f>'Summary Qty'!N73</f>
         <v>226.06215610510046</v>
       </c>
-      <c r="E73" s="1">
-        <f>'Summary Qty'!O73</f>
-        <v>29</v>
+      <c r="E73" s="12">
+        <v>45</v>
       </c>
       <c r="F73" s="1">
         <f t="shared" si="0"/>
@@ -3658,7 +3622,7 @@
         <v>3.2283012748546773E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <f>'Summary Qty'!A74</f>
         <v>533</v>
@@ -3675,9 +3639,8 @@
         <f>'Summary Qty'!N74</f>
         <v>251.74445463812432</v>
       </c>
-      <c r="E74" s="1">
-        <f>'Summary Qty'!O74</f>
-        <v>52</v>
+      <c r="E74" s="12">
+        <v>60</v>
       </c>
       <c r="F74" s="1">
         <f t="shared" si="0"/>
@@ -3695,7 +3658,7 @@
         <v>2.4474216001796278E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <f>'Summary Qty'!A75</f>
         <v>534</v>
@@ -3712,9 +3675,8 @@
         <f>'Summary Qty'!N75</f>
         <v>283.9324431818182</v>
       </c>
-      <c r="E75" s="1">
-        <f>'Summary Qty'!O75</f>
-        <v>58</v>
+      <c r="E75" s="12">
+        <v>30</v>
       </c>
       <c r="F75" s="1">
         <f t="shared" si="0"/>
@@ -3732,7 +3694,7 @@
         <v>1.3172666716563135E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <f>'Summary Qty'!A76</f>
         <v>535</v>
@@ -3749,9 +3711,8 @@
         <f>'Summary Qty'!N76</f>
         <v>328.42972222222227</v>
       </c>
-      <c r="E76" s="1">
-        <f>'Summary Qty'!O76</f>
-        <v>22</v>
+      <c r="E76" s="12">
+        <v>45</v>
       </c>
       <c r="F76" s="1">
         <f t="shared" si="0"/>
@@ -3769,7 +3730,7 @@
         <v>5.3888182022303732E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <f>'Summary Qty'!A77</f>
         <v>572</v>
@@ -3786,9 +3747,8 @@
         <f>'Summary Qty'!N77</f>
         <v>103.86861111111111</v>
       </c>
-      <c r="E77" s="1">
-        <f>'Summary Qty'!O77</f>
-        <v>32</v>
+      <c r="E77" s="12">
+        <v>30</v>
       </c>
       <c r="F77" s="1">
         <f t="shared" si="0"/>
@@ -3806,7 +3766,7 @@
         <v>8.9813636703839567E-4</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <f>'Summary Qty'!A78</f>
         <v>574</v>
@@ -3823,9 +3783,8 @@
         <f>'Summary Qty'!N78</f>
         <v>117.72857142857143</v>
       </c>
-      <c r="E78" s="1">
-        <f>'Summary Qty'!O78</f>
-        <v>35</v>
+      <c r="E78" s="11">
+        <v>31</v>
       </c>
       <c r="F78" s="1">
         <f t="shared" si="0"/>
@@ -3843,7 +3802,7 @@
         <v>1.7463762692413248E-4</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <f>'Summary Qty'!A79</f>
         <v>576</v>
@@ -3860,9 +3819,8 @@
         <f>'Summary Qty'!N79</f>
         <v>208.25</v>
       </c>
-      <c r="E79" s="1">
-        <f>'Summary Qty'!O79</f>
-        <v>26</v>
+      <c r="E79" s="11">
+        <v>31.52</v>
       </c>
       <c r="F79" s="1">
         <f t="shared" si="0"/>
@@ -3880,7 +3838,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <f>'Summary Qty'!A80</f>
         <v>577</v>
@@ -3897,9 +3855,8 @@
         <f>'Summary Qty'!N80</f>
         <v>32.037417102966842</v>
       </c>
-      <c r="E80" s="1">
-        <f>'Summary Qty'!O80</f>
-        <v>33</v>
+      <c r="E80" s="12">
+        <v>30</v>
       </c>
       <c r="F80" s="1">
         <f t="shared" si="0"/>
@@ -3917,7 +3874,7 @@
         <v>1.4295337175361128E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <f>'Summary Qty'!A81</f>
         <v>578</v>
@@ -3934,8 +3891,7 @@
         <f>'Summary Qty'!N81</f>
         <v>43.177956989247313</v>
       </c>
-      <c r="E81" s="1">
-        <f>'Summary Qty'!O81</f>
+      <c r="E81" s="12">
         <v>30</v>
       </c>
       <c r="F81" s="1">
@@ -3954,7 +3910,7 @@
         <v>2.3201856148491887E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <f>'Summary Qty'!A82</f>
         <v>88521</v>
@@ -3971,9 +3927,8 @@
         <f>'Summary Qty'!N82</f>
         <v>117.44166666666666</v>
       </c>
-      <c r="E82" s="1">
-        <f>'Summary Qty'!O82</f>
-        <v>51</v>
+      <c r="E82" s="12">
+        <v>15</v>
       </c>
       <c r="F82" s="1">
         <f t="shared" si="0"/>
@@ -3991,7 +3946,7 @@
         <v>1.4968939450639928E-4</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <f>'Summary Qty'!A83</f>
         <v>88523</v>
@@ -4008,9 +3963,8 @@
         <f>'Summary Qty'!N83</f>
         <v>169.03</v>
       </c>
-      <c r="E83" s="1">
-        <f>'Summary Qty'!O83</f>
-        <v>57</v>
+      <c r="E83" s="12">
+        <v>25</v>
       </c>
       <c r="F83" s="1">
         <f t="shared" si="0"/>
@@ -4028,7 +3982,7 @@
         <v>1.2474116208866605E-4</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <f>'Summary Qty'!A84</f>
         <v>88524</v>
@@ -4045,9 +3999,8 @@
         <f>'Summary Qty'!N84</f>
         <v>195.61250000000001</v>
       </c>
-      <c r="E84" s="1">
-        <f>'Summary Qty'!O84</f>
-        <v>44</v>
+      <c r="E84" s="12">
+        <v>25</v>
       </c>
       <c r="F84" s="1">
         <f t="shared" si="0"/>
@@ -4065,7 +4018,7 @@
         <v>1.9958585934186569E-4</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <f>'Summary Qty'!A85</f>
         <v>88525</v>
@@ -4082,9 +4035,8 @@
         <f>'Summary Qty'!N85</f>
         <v>229.85</v>
       </c>
-      <c r="E85" s="1">
-        <f>'Summary Qty'!O85</f>
-        <v>20</v>
+      <c r="E85" s="12">
+        <v>25</v>
       </c>
       <c r="F85" s="1">
         <f t="shared" si="0"/>
@@ -4102,7 +4054,7 @@
         <v>9.9792929670932843E-5</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <f>'Summary Qty'!A86</f>
         <v>88531</v>
@@ -4119,9 +4071,8 @@
         <f>'Summary Qty'!N86</f>
         <v>124.69272727272728</v>
       </c>
-      <c r="E86" s="1">
-        <f>'Summary Qty'!O86</f>
-        <v>23</v>
+      <c r="E86" s="12">
+        <v>30</v>
       </c>
       <c r="F86" s="1">
         <f t="shared" si="0"/>
@@ -4139,7 +4090,7 @@
         <v>1.3721527829753267E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <f>'Summary Qty'!A87</f>
         <v>88532</v>
@@ -4156,9 +4107,8 @@
         <f>'Summary Qty'!N87</f>
         <v>156.70848484848483</v>
       </c>
-      <c r="E87" s="1">
-        <f>'Summary Qty'!O87</f>
-        <v>22</v>
+      <c r="E87" s="12">
+        <v>45</v>
       </c>
       <c r="F87" s="1">
         <f t="shared" si="0"/>
@@ -4176,7 +4126,7 @@
         <v>4.11645834892598E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <f>'Summary Qty'!A88</f>
         <v>88533</v>
@@ -4193,9 +4143,8 @@
         <f>'Summary Qty'!N88</f>
         <v>190.20784313725491</v>
       </c>
-      <c r="E88" s="1">
-        <f>'Summary Qty'!O88</f>
-        <v>45</v>
+      <c r="E88" s="12">
+        <v>60</v>
       </c>
       <c r="F88" s="1">
         <f t="shared" si="0"/>
@@ -4213,7 +4162,7 @@
         <v>1.272359853304394E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <f>'Summary Qty'!A89</f>
         <v>88534</v>
@@ -4230,9 +4179,8 @@
         <f>'Summary Qty'!N89</f>
         <v>213.35555555555555</v>
       </c>
-      <c r="E89" s="1">
-        <f>'Summary Qty'!O89</f>
-        <v>24</v>
+      <c r="E89" s="12">
+        <v>30</v>
       </c>
       <c r="F89" s="1">
         <f t="shared" si="0"/>
@@ -4250,7 +4198,7 @@
         <v>2.2453409175959892E-4</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <f>'Summary Qty'!A90</f>
         <v>88586</v>
@@ -4267,9 +4215,8 @@
         <f>'Summary Qty'!N90</f>
         <v>259.73</v>
       </c>
-      <c r="E90" s="1">
-        <f>'Summary Qty'!O90</f>
-        <v>33</v>
+      <c r="E90" s="12">
+        <v>30</v>
       </c>
       <c r="F90" s="1">
         <f t="shared" si="0"/>
@@ -4287,7 +4234,7 @@
         <v>1.2474116208866605E-4</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <f>'Summary Qty'!A91</f>
         <v>613</v>
@@ -4304,9 +4251,8 @@
         <f>'Summary Qty'!N91</f>
         <v>1526.7855555555554</v>
       </c>
-      <c r="E91" s="1">
-        <f>'Summary Qty'!O91</f>
-        <v>25</v>
+      <c r="E91" s="12">
+        <v>45</v>
       </c>
       <c r="F91" s="1">
         <f t="shared" si="0"/>
@@ -4324,7 +4270,7 @@
         <v>6.7360227527879669E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <f>'Summary Qty'!A92</f>
         <v>627</v>
@@ -4341,9 +4287,8 @@
         <f>'Summary Qty'!N92</f>
         <v>229.51827411167511</v>
       </c>
-      <c r="E92" s="1">
-        <f>'Summary Qty'!O92</f>
-        <v>53</v>
+      <c r="E92" s="11">
+        <v>24</v>
       </c>
       <c r="F92" s="1">
         <f t="shared" si="0"/>
@@ -4361,7 +4306,7 @@
         <v>4.9148017862934426E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <f>'Summary Qty'!A93</f>
         <v>642</v>
@@ -4378,9 +4323,8 @@
         <f>'Summary Qty'!N93</f>
         <v>415</v>
       </c>
-      <c r="E93" s="1">
-        <f>'Summary Qty'!O93</f>
-        <v>47</v>
+      <c r="E93" s="11">
+        <v>24</v>
       </c>
       <c r="F93" s="1">
         <f t="shared" si="0"/>
@@ -4398,7 +4342,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <f>'Summary Qty'!A94</f>
         <v>643</v>
@@ -4415,9 +4359,8 @@
         <f>'Summary Qty'!N94</f>
         <v>1181</v>
       </c>
-      <c r="E94" s="1">
-        <f>'Summary Qty'!O94</f>
-        <v>56</v>
+      <c r="E94" s="11">
+        <v>24</v>
       </c>
       <c r="F94" s="1">
         <f t="shared" si="0"/>
@@ -4435,7 +4378,7 @@
         <v>4.241199511014646E-4</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <f>'Summary Qty'!A95</f>
         <v>651</v>
@@ -4452,9 +4395,8 @@
         <f>'Summary Qty'!N95</f>
         <v>188.6</v>
       </c>
-      <c r="E95" s="1">
-        <f>'Summary Qty'!O95</f>
-        <v>58</v>
+      <c r="E95" s="12">
+        <v>10</v>
       </c>
       <c r="F95" s="1">
         <f t="shared" si="0"/>
@@ -4472,7 +4414,7 @@
         <v>1.2474116208866605E-4</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <f>'Summary Qty'!A96</f>
         <v>652</v>
@@ -4489,9 +4431,8 @@
         <f>'Summary Qty'!N96</f>
         <v>167</v>
       </c>
-      <c r="E96" s="1">
-        <f>'Summary Qty'!O96</f>
-        <v>44</v>
+      <c r="E96" s="12">
+        <v>10</v>
       </c>
       <c r="F96" s="1">
         <f t="shared" si="0"/>
@@ -4509,7 +4450,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <f>'Summary Qty'!A97</f>
         <v>655</v>
@@ -4526,9 +4467,8 @@
         <f>'Summary Qty'!N97</f>
         <v>62.663636363636357</v>
       </c>
-      <c r="E97" s="1">
-        <f>'Summary Qty'!O97</f>
-        <v>48</v>
+      <c r="E97" s="12">
+        <v>10</v>
       </c>
       <c r="F97" s="1">
         <f t="shared" si="0"/>
@@ -4546,7 +4486,7 @@
         <v>2.7443055659506533E-4</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <f>'Summary Qty'!A98</f>
         <v>711</v>
@@ -4563,9 +4503,8 @@
         <f>'Summary Qty'!N98</f>
         <v>1372.5</v>
       </c>
-      <c r="E98" s="1">
-        <f>'Summary Qty'!O98</f>
-        <v>48</v>
+      <c r="E98" s="12">
+        <v>30</v>
       </c>
       <c r="F98" s="1">
         <f t="shared" si="0"/>
@@ -4583,7 +4522,7 @@
         <v>3.4927525384826496E-4</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <f>'Summary Qty'!A99</f>
         <v>712</v>
@@ -4600,9 +4539,8 @@
         <f>'Summary Qty'!N99</f>
         <v>1391.5</v>
       </c>
-      <c r="E99" s="1">
-        <f>'Summary Qty'!O99</f>
-        <v>56</v>
+      <c r="E99" s="12">
+        <v>30</v>
       </c>
       <c r="F99" s="1">
         <f t="shared" si="0"/>
@@ -4620,7 +4558,7 @@
         <v>1.4968939450639928E-4</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <f>'Summary Qty'!A100</f>
         <v>721</v>
@@ -4637,9 +4575,8 @@
         <f>'Summary Qty'!N100</f>
         <v>836.63888888888891</v>
       </c>
-      <c r="E100" s="1">
-        <f>'Summary Qty'!O100</f>
-        <v>43</v>
+      <c r="E100" s="12">
+        <v>30</v>
       </c>
       <c r="F100" s="1">
         <f t="shared" si="0"/>
@@ -4657,7 +4594,7 @@
         <v>2.2453409175959892E-4</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <f>'Summary Qty'!A101</f>
         <v>722</v>
@@ -4674,9 +4611,8 @@
         <f>'Summary Qty'!N101</f>
         <v>921.66666666666663</v>
       </c>
-      <c r="E101" s="1">
-        <f>'Summary Qty'!O101</f>
-        <v>39</v>
+      <c r="E101" s="12">
+        <v>30</v>
       </c>
       <c r="F101" s="1">
         <f t="shared" si="0"/>
@@ -4694,7 +4630,7 @@
         <v>7.4844697253199639E-5</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <f>'Summary Qty'!A102</f>
         <v>727</v>
@@ -4711,9 +4647,8 @@
         <f>'Summary Qty'!N102</f>
         <v>1379.78</v>
       </c>
-      <c r="E102" s="1">
-        <f>'Summary Qty'!O102</f>
-        <v>48</v>
+      <c r="E102" s="11">
+        <v>24</v>
       </c>
       <c r="F102" s="1">
         <f t="shared" si="0"/>
@@ -4731,7 +4666,7 @@
         <v>1.2474116208866605E-4</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <f>'Summary Qty'!A103</f>
         <v>728</v>
@@ -4748,9 +4683,8 @@
         <f>'Summary Qty'!N103</f>
         <v>1564.19</v>
       </c>
-      <c r="E103" s="1">
-        <f>'Summary Qty'!O103</f>
-        <v>44</v>
+      <c r="E103" s="11">
+        <v>24</v>
       </c>
       <c r="F103" s="1">
         <f t="shared" si="0"/>
@@ -4768,7 +4702,7 @@
         <v>1.2474116208866605E-4</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <f>'Summary Qty'!A104</f>
         <v>731</v>
@@ -4785,9 +4719,8 @@
         <f>'Summary Qty'!N104</f>
         <v>53.979310344827589</v>
       </c>
-      <c r="E104" s="1">
-        <f>'Summary Qty'!O104</f>
-        <v>24</v>
+      <c r="E104" s="12">
+        <v>30</v>
       </c>
       <c r="F104" s="1">
         <f t="shared" si="0"/>
@@ -4805,7 +4738,7 @@
         <v>7.2349874011426321E-4</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <f>'Summary Qty'!A105</f>
         <v>732</v>
@@ -4822,9 +4755,8 @@
         <f>'Summary Qty'!N105</f>
         <v>53.2</v>
       </c>
-      <c r="E105" s="1">
-        <f>'Summary Qty'!O105</f>
-        <v>22</v>
+      <c r="E105" s="12">
+        <v>30</v>
       </c>
       <c r="F105" s="1">
         <f t="shared" si="0"/>
@@ -4842,7 +4774,7 @@
         <v>2.2453409175959892E-4</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <f>'Summary Qty'!A106</f>
         <v>733</v>
@@ -4859,8 +4791,7 @@
         <f>'Summary Qty'!N106</f>
         <v>49.126984126984127</v>
       </c>
-      <c r="E106" s="1">
-        <f>'Summary Qty'!O106</f>
+      <c r="E106" s="11">
         <v>24</v>
       </c>
       <c r="F106" s="1">
@@ -4879,7 +4810,7 @@
         <v>1.5717386423171923E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <f>'Summary Qty'!A107</f>
         <v>736</v>
@@ -4896,9 +4827,8 @@
         <f>'Summary Qty'!N107</f>
         <v>47.3046875</v>
       </c>
-      <c r="E107" s="1">
-        <f>'Summary Qty'!O107</f>
-        <v>27</v>
+      <c r="E107" s="11">
+        <v>24</v>
       </c>
       <c r="F107" s="1">
         <f t="shared" si="0"/>
@@ -4916,7 +4846,7 @@
         <v>7.9834343736746275E-4</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <f>'Summary Qty'!A108</f>
         <v>741</v>
@@ -4933,9 +4863,8 @@
         <f>'Summary Qty'!N108</f>
         <v>48.137500000000003</v>
       </c>
-      <c r="E108" s="1">
-        <f>'Summary Qty'!O108</f>
-        <v>26</v>
+      <c r="E108" s="12">
+        <v>30</v>
       </c>
       <c r="F108" s="1">
         <f t="shared" si="0"/>
@@ -4953,7 +4882,7 @@
         <v>9.9792929670932843E-5</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <f>'Summary Qty'!A109</f>
         <v>743</v>
@@ -4970,9 +4899,8 @@
         <f>'Summary Qty'!N109</f>
         <v>440.2</v>
       </c>
-      <c r="E109" s="1">
-        <f>'Summary Qty'!O109</f>
-        <v>38</v>
+      <c r="E109" s="12">
+        <v>30</v>
       </c>
       <c r="F109" s="1">
         <f t="shared" si="0"/>
@@ -4990,7 +4918,7 @@
         <v>2.4948232417733209E-4</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <f>'Summary Qty'!A110</f>
         <v>744</v>
@@ -5007,9 +4935,8 @@
         <f>'Summary Qty'!N110</f>
         <v>443.5</v>
       </c>
-      <c r="E110" s="1">
-        <f>'Summary Qty'!O110</f>
-        <v>34</v>
+      <c r="E110" s="12">
+        <v>30</v>
       </c>
       <c r="F110" s="1">
         <f t="shared" si="0"/>
@@ -5027,7 +4954,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <f>'Summary Qty'!A111</f>
         <v>811</v>
@@ -5044,9 +4971,8 @@
         <f>'Summary Qty'!N111</f>
         <v>265.1192660550459</v>
       </c>
-      <c r="E111" s="1">
-        <f>'Summary Qty'!O111</f>
-        <v>43</v>
+      <c r="E111" s="11">
+        <v>20</v>
       </c>
       <c r="F111" s="1">
         <f t="shared" si="0"/>
@@ -5064,7 +4990,7 @@
         <v>2.7193573335329204E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <f>'Summary Qty'!A112</f>
         <v>825</v>
@@ -5081,9 +5007,8 @@
         <f>'Summary Qty'!N112</f>
         <v>1860.1550420168069</v>
       </c>
-      <c r="E112" s="1">
-        <f>'Summary Qty'!O112</f>
-        <v>16</v>
+      <c r="E112" s="11">
+        <v>20</v>
       </c>
       <c r="F112" s="1">
         <f t="shared" si="0"/>
@@ -5101,7 +5026,7 @@
         <v>2.9688396577102522E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <f>'Summary Qty'!A113</f>
         <v>833</v>
@@ -5118,9 +5043,8 @@
         <f>'Summary Qty'!N113</f>
         <v>725</v>
       </c>
-      <c r="E113" s="1">
-        <f>'Summary Qty'!O113</f>
-        <v>18</v>
+      <c r="E113" s="11">
+        <v>40</v>
       </c>
       <c r="F113" s="1">
         <f t="shared" si="0"/>
@@ -5138,7 +5062,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <f>'Summary Qty'!A114</f>
         <v>845</v>
@@ -5155,9 +5079,8 @@
         <f>'Summary Qty'!N114</f>
         <v>344</v>
       </c>
-      <c r="E114" s="1">
-        <f>'Summary Qty'!O114</f>
-        <v>52</v>
+      <c r="E114" s="11">
+        <v>20</v>
       </c>
       <c r="F114" s="1">
         <f t="shared" si="0"/>
@@ -5175,7 +5098,7 @@
         <v>3.742234862659982E-4</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <f>'Summary Qty'!A115</f>
         <v>846</v>
@@ -5192,9 +5115,8 @@
         <f>'Summary Qty'!N115</f>
         <v>202.5</v>
       </c>
-      <c r="E115" s="1">
-        <f>'Summary Qty'!O115</f>
-        <v>46</v>
+      <c r="E115" s="11">
+        <v>20</v>
       </c>
       <c r="F115" s="1">
         <f t="shared" si="0"/>
@@ -5212,7 +5134,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <f>'Summary Qty'!A116</f>
         <v>872</v>
@@ -5229,9 +5151,8 @@
         <f>'Summary Qty'!N116</f>
         <v>179</v>
       </c>
-      <c r="E116" s="1">
-        <f>'Summary Qty'!O116</f>
-        <v>28</v>
+      <c r="E116" s="11">
+        <v>20</v>
       </c>
       <c r="F116" s="1">
         <f t="shared" si="0"/>
@@ -5249,7 +5170,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <f>'Summary Qty'!A117</f>
         <v>874</v>
@@ -5266,9 +5187,8 @@
         <f>'Summary Qty'!N117</f>
         <v>140.79444444444445</v>
       </c>
-      <c r="E117" s="1">
-        <f>'Summary Qty'!O117</f>
-        <v>60</v>
+      <c r="E117" s="12">
+        <v>30</v>
       </c>
       <c r="F117" s="1">
         <f t="shared" si="0"/>
@@ -5286,7 +5206,7 @@
         <v>2.2453409175959892E-4</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <f>'Summary Qty'!A118</f>
         <v>88943</v>
@@ -5303,9 +5223,8 @@
         <f>'Summary Qty'!N118</f>
         <v>67.864285714285714</v>
       </c>
-      <c r="E118" s="1">
-        <f>'Summary Qty'!O118</f>
-        <v>47</v>
+      <c r="E118" s="11">
+        <v>18</v>
       </c>
       <c r="F118" s="1">
         <f t="shared" si="0"/>
@@ -5323,7 +5242,7 @@
         <v>1.2224633884689274E-3</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <f>'Summary Qty'!A119</f>
         <v>915</v>
@@ -5340,9 +5259,8 @@
         <f>'Summary Qty'!N119</f>
         <v>187</v>
       </c>
-      <c r="E119" s="1">
-        <f>'Summary Qty'!O119</f>
-        <v>45</v>
+      <c r="E119" s="12">
+        <v>30</v>
       </c>
       <c r="F119" s="1">
         <f t="shared" si="0"/>
@@ -5360,7 +5278,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <f>'Summary Qty'!A120</f>
         <v>916</v>
@@ -5377,9 +5295,8 @@
         <f>'Summary Qty'!N120</f>
         <v>109</v>
       </c>
-      <c r="E120" s="1">
-        <f>'Summary Qty'!O120</f>
-        <v>35</v>
+      <c r="E120" s="11">
+        <v>18</v>
       </c>
       <c r="F120" s="1">
         <f t="shared" si="0"/>
@@ -5397,7 +5314,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <f>'Summary Qty'!A121</f>
         <v>926</v>
@@ -5414,9 +5331,8 @@
         <f>'Summary Qty'!N121</f>
         <v>152.91</v>
       </c>
-      <c r="E121" s="1">
-        <f>'Summary Qty'!O121</f>
-        <v>57</v>
+      <c r="E121" s="12">
+        <v>15</v>
       </c>
       <c r="F121" s="1">
         <f t="shared" si="0"/>
@@ -5434,7 +5350,7 @@
         <v>4.9896464835466423E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <f>'Summary Qty'!A122</f>
         <v>927</v>
@@ -5451,9 +5367,8 @@
         <f>'Summary Qty'!N122</f>
         <v>13.027037037037037</v>
       </c>
-      <c r="E122" s="1">
-        <f>'Summary Qty'!O122</f>
-        <v>16</v>
+      <c r="E122" s="12">
+        <v>15</v>
       </c>
       <c r="F122" s="1">
         <f t="shared" si="0"/>
@@ -5471,7 +5386,7 @@
         <v>1.0104034129181951E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <f>'Summary Qty'!A123</f>
         <v>943</v>
@@ -5488,9 +5403,8 @@
         <f>'Summary Qty'!N123</f>
         <v>84.456140350877192</v>
       </c>
-      <c r="E123" s="1">
-        <f>'Summary Qty'!O123</f>
-        <v>27</v>
+      <c r="E123" s="11">
+        <v>18</v>
       </c>
       <c r="F123" s="1">
         <f t="shared" si="0"/>
@@ -5508,7 +5422,7 @@
         <v>2.8440984956215861E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <f>'Summary Qty'!A124</f>
         <v>945</v>
@@ -5525,9 +5439,8 @@
         <f>'Summary Qty'!N124</f>
         <v>200</v>
       </c>
-      <c r="E124" s="1">
-        <f>'Summary Qty'!O124</f>
-        <v>36</v>
+      <c r="E124" s="12">
+        <v>5</v>
       </c>
       <c r="F124" s="1">
         <f t="shared" si="0"/>
@@ -5545,7 +5458,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <f>'Summary Qty'!A125</f>
         <v>949</v>
@@ -5562,9 +5475,8 @@
         <f>'Summary Qty'!N125</f>
         <v>224</v>
       </c>
-      <c r="E125" s="1">
-        <f>'Summary Qty'!O125</f>
-        <v>19</v>
+      <c r="E125" s="11">
+        <v>18</v>
       </c>
       <c r="F125" s="1">
         <f t="shared" si="0"/>
@@ -5582,7 +5494,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <f>'Summary Qty'!A126</f>
         <v>965</v>
@@ -5599,9 +5511,8 @@
         <f>'Summary Qty'!N126</f>
         <v>540.97676056338025</v>
       </c>
-      <c r="E126" s="1">
-        <f>'Summary Qty'!O126</f>
-        <v>35</v>
+      <c r="E126" s="12">
+        <v>30</v>
       </c>
       <c r="F126" s="1">
         <f t="shared" si="0"/>
@@ -5619,8 +5530,8 @@
         <v>1.7713245016590582E-3</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A127" s="1">
+    <row r="127" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="14">
         <f>'Summary Qty'!A127</f>
         <v>0</v>
       </c>
@@ -5636,9 +5547,8 @@
         <f>'Summary Qty'!N127</f>
         <v>214.375</v>
       </c>
-      <c r="E127" s="1">
-        <f>'Summary Qty'!O127</f>
-        <v>32</v>
+      <c r="E127" s="11">
+        <v>22.5</v>
       </c>
       <c r="F127" s="1">
         <f t="shared" si="0"/>
@@ -5656,7 +5566,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <f>'Summary Qty'!A128</f>
         <v>981</v>
@@ -5673,9 +5583,8 @@
         <f>'Summary Qty'!N128</f>
         <v>400</v>
       </c>
-      <c r="E128" s="1">
-        <f>'Summary Qty'!O128</f>
-        <v>44</v>
+      <c r="E128" s="12">
+        <v>30</v>
       </c>
       <c r="F128" s="1">
         <f t="shared" si="0"/>
@@ -5693,7 +5602,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <f>'Summary Qty'!A129</f>
         <v>990</v>
@@ -5710,9 +5619,8 @@
         <f>'Summary Qty'!N129</f>
         <v>116.27272727272727</v>
       </c>
-      <c r="E129" s="1">
-        <f>'Summary Qty'!O129</f>
-        <v>24</v>
+      <c r="E129" s="12">
+        <v>15</v>
       </c>
       <c r="F129" s="1">
         <f t="shared" si="0"/>
@@ -5730,7 +5638,7 @@
         <v>5.4886111319013065E-4</v>
       </c>
     </row>
-    <row r="130" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <f>'Summary Qty'!A130</f>
         <v>9999</v>
@@ -5747,9 +5655,8 @@
         <f>'Summary Qty'!N130</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="E130" s="1">
-        <f>'Summary Qty'!O130</f>
-        <v>53</v>
+      <c r="E130" s="11">
+        <v>22.5</v>
       </c>
       <c r="F130" s="1">
         <f t="shared" si="0"/>
@@ -5767,7 +5674,7 @@
         <v>2.2079185689693893E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="str">
         <f>'Summary Qty'!A131</f>
         <v>Cem</v>
@@ -5784,9 +5691,8 @@
         <f>'Summary Qty'!N131</f>
         <v>1.4193548387096775</v>
       </c>
-      <c r="E131" s="1">
-        <f>'Summary Qty'!O131</f>
-        <v>38</v>
+      <c r="E131" s="11">
+        <v>22.5</v>
       </c>
       <c r="F131" s="1">
         <f t="shared" si="0"/>
@@ -5804,7 +5710,7 @@
         <v>3.8669760247486478E-3</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="str">
         <f>'Summary Qty'!A132</f>
         <v>D9986</v>
@@ -5821,9 +5727,8 @@
         <f>'Summary Qty'!N132</f>
         <v>0.54780564263322884</v>
       </c>
-      <c r="E132" s="1">
-        <f>'Summary Qty'!O132</f>
-        <v>33</v>
+      <c r="E132" s="11">
+        <v>22.5</v>
       </c>
       <c r="F132" s="1">
         <f t="shared" si="0"/>
@@ -5841,7 +5746,7 @@
         <v>3.1833944565027576E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="str">
         <f>'Summary Qty'!A133</f>
         <v>Insert</v>
@@ -5858,9 +5763,8 @@
         <f>'Summary Qty'!N133</f>
         <v>0</v>
       </c>
-      <c r="E133" s="1">
-        <f>'Summary Qty'!O133</f>
-        <v>27</v>
+      <c r="E133" s="11">
+        <v>22.5</v>
       </c>
       <c r="F133" s="1">
         <f t="shared" si="0"/>
@@ -5878,7 +5782,7 @@
         <v>3.4927525384826496E-4</v>
       </c>
     </row>
-    <row r="134" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="str">
         <f>'Summary Qty'!A134</f>
         <v>Zclin</v>
@@ -5895,9 +5799,8 @@
         <f>'Summary Qty'!N134</f>
         <v>0</v>
       </c>
-      <c r="E134" s="1">
-        <f>'Summary Qty'!O134</f>
-        <v>21</v>
+      <c r="E134" s="11">
+        <v>12.5</v>
       </c>
       <c r="F134" s="1">
         <f t="shared" si="0"/>
@@ -5915,7 +5818,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="135" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <f>'Summary Qty'!A135</f>
         <v>15</v>
@@ -5932,9 +5835,8 @@
         <f>'Summary Qty'!N135</f>
         <v>99.166666666666671</v>
       </c>
-      <c r="E135" s="1">
-        <f>'Summary Qty'!O135</f>
-        <v>39</v>
+      <c r="E135" s="11">
+        <v>30</v>
       </c>
       <c r="F135" s="1">
         <f t="shared" si="0"/>
@@ -5952,7 +5854,7 @@
         <v>1.4968939450639928E-4</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <f>'Summary Qty'!A136</f>
         <v>19</v>
@@ -5969,9 +5871,8 @@
         <f>'Summary Qty'!N136</f>
         <v>59.085000000000001</v>
       </c>
-      <c r="E136" s="1">
-        <f>'Summary Qty'!O136</f>
-        <v>25</v>
+      <c r="E136" s="11">
+        <v>15</v>
       </c>
       <c r="F136" s="1">
         <f t="shared" si="0"/>
@@ -5989,7 +5890,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <f>'Summary Qty'!A137</f>
         <v>316</v>
@@ -6006,9 +5907,8 @@
         <f>'Summary Qty'!N137</f>
         <v>77.28</v>
       </c>
-      <c r="E137" s="1">
-        <f>'Summary Qty'!O137</f>
-        <v>35</v>
+      <c r="E137" s="11">
+        <v>17.37</v>
       </c>
       <c r="F137" s="1">
         <f t="shared" si="0"/>
@@ -6026,7 +5926,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <f>'Summary Qty'!A138</f>
         <v>165</v>
@@ -6043,9 +5943,8 @@
         <f>'Summary Qty'!N138</f>
         <v>25.27</v>
       </c>
-      <c r="E138" s="1">
-        <f>'Summary Qty'!O138</f>
-        <v>42</v>
+      <c r="E138" s="11">
+        <v>15</v>
       </c>
       <c r="F138" s="1">
         <f t="shared" si="0"/>
@@ -6063,7 +5962,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <f>'Summary Qty'!A139</f>
         <v>88322</v>
@@ -6080,9 +5979,8 @@
         <f>'Summary Qty'!N139</f>
         <v>218.65</v>
       </c>
-      <c r="E139" s="1">
-        <f>'Summary Qty'!O139</f>
-        <v>25</v>
+      <c r="E139" s="11">
+        <v>45</v>
       </c>
       <c r="F139" s="1">
         <f t="shared" si="0"/>
@@ -6100,7 +5998,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <f>'Summary Qty'!A140</f>
         <v>556</v>
@@ -6117,9 +6015,8 @@
         <f>'Summary Qty'!N140</f>
         <v>1396.3636363636363</v>
       </c>
-      <c r="E140" s="1">
-        <f>'Summary Qty'!O140</f>
-        <v>53</v>
+      <c r="E140" s="11">
+        <v>75</v>
       </c>
       <c r="F140" s="1">
         <f t="shared" si="0"/>
@@ -6137,7 +6034,7 @@
         <v>5.4886111319013065E-4</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <f>'Summary Qty'!A141</f>
         <v>631</v>
@@ -6154,9 +6051,8 @@
         <f>'Summary Qty'!N141</f>
         <v>35</v>
       </c>
-      <c r="E141" s="1">
-        <f>'Summary Qty'!O141</f>
-        <v>20</v>
+      <c r="E141" s="11">
+        <v>15</v>
       </c>
       <c r="F141" s="1">
         <f t="shared" si="0"/>
@@ -6174,7 +6070,7 @@
         <v>9.9792929670932843E-5</v>
       </c>
     </row>
-    <row r="142" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <f>'Summary Qty'!A142</f>
         <v>656</v>
@@ -6191,9 +6087,8 @@
         <f>'Summary Qty'!N142</f>
         <v>165</v>
       </c>
-      <c r="E142" s="1">
-        <f>'Summary Qty'!O142</f>
-        <v>41</v>
+      <c r="E142" s="12">
+        <v>10</v>
       </c>
       <c r="F142" s="1">
         <f t="shared" si="0"/>
@@ -6211,7 +6106,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <f>'Summary Qty'!A143</f>
         <v>753</v>
@@ -6228,9 +6123,8 @@
         <f>'Summary Qty'!N143</f>
         <v>0</v>
       </c>
-      <c r="E143" s="1">
-        <f>'Summary Qty'!O143</f>
-        <v>31</v>
+      <c r="E143" s="12">
+        <v>30</v>
       </c>
       <c r="F143" s="1">
         <f t="shared" si="0"/>
@@ -6248,7 +6142,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="144" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <f>'Summary Qty'!A144</f>
         <v>768</v>
@@ -6265,9 +6159,8 @@
         <f>'Summary Qty'!N144</f>
         <v>196.11111111111111</v>
       </c>
-      <c r="E144" s="1">
-        <f>'Summary Qty'!O144</f>
-        <v>17</v>
+      <c r="E144" s="12">
+        <v>30</v>
       </c>
       <c r="F144" s="1">
         <f t="shared" si="0"/>
@@ -6285,7 +6178,7 @@
         <v>2.2453409175959892E-4</v>
       </c>
     </row>
-    <row r="145" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <f>'Summary Qty'!A145</f>
         <v>776</v>
@@ -6302,9 +6195,8 @@
         <f>'Summary Qty'!N145</f>
         <v>70</v>
       </c>
-      <c r="E145" s="1">
-        <f>'Summary Qty'!O145</f>
-        <v>57</v>
+      <c r="E145" s="12">
+        <v>15</v>
       </c>
       <c r="F145" s="1">
         <f t="shared" si="0"/>
@@ -6322,7 +6214,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="146" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <f>'Summary Qty'!A146</f>
         <v>823</v>
@@ -6339,9 +6231,8 @@
         <f>'Summary Qty'!N146</f>
         <v>950</v>
       </c>
-      <c r="E146" s="1">
-        <f>'Summary Qty'!O146</f>
-        <v>45</v>
+      <c r="E146" s="11">
+        <v>37.5</v>
       </c>
       <c r="F146" s="1">
         <f t="shared" si="0"/>
@@ -6359,7 +6250,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="147" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <f>'Summary Qty'!A147</f>
         <v>841</v>
@@ -6376,9 +6267,8 @@
         <f>'Summary Qty'!N147</f>
         <v>310.25</v>
       </c>
-      <c r="E147" s="1">
-        <f>'Summary Qty'!O147</f>
-        <v>36</v>
+      <c r="E147" s="11">
+        <v>37.5</v>
       </c>
       <c r="F147" s="1">
         <f t="shared" si="0"/>
@@ -6396,7 +6286,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="148" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <f>'Summary Qty'!A148</f>
         <v>873</v>
@@ -6413,9 +6303,8 @@
         <f>'Summary Qty'!N148</f>
         <v>180.5</v>
       </c>
-      <c r="E148" s="1">
-        <f>'Summary Qty'!O148</f>
-        <v>49</v>
+      <c r="E148" s="11">
+        <v>25</v>
       </c>
       <c r="F148" s="1">
         <f t="shared" si="0"/>
@@ -6433,7 +6322,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="149" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <f>'Summary Qty'!A149</f>
         <v>966</v>
@@ -6450,9 +6339,8 @@
         <f>'Summary Qty'!N149</f>
         <v>70.3</v>
       </c>
-      <c r="E149" s="1">
-        <f>'Summary Qty'!O149</f>
-        <v>28</v>
+      <c r="E149" s="12">
+        <v>15</v>
       </c>
       <c r="F149" s="1">
         <f t="shared" si="0"/>
@@ -6470,7 +6358,7 @@
         <v>1.2474116208866605E-4</v>
       </c>
     </row>
-    <row r="150" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="str">
         <f>'Summary Qty'!A150</f>
         <v>Script</v>
@@ -6487,9 +6375,8 @@
         <f>'Summary Qty'!N150</f>
         <v>0.55555555555555558</v>
       </c>
-      <c r="E150" s="1">
-        <f>'Summary Qty'!O150</f>
-        <v>28</v>
+      <c r="E150" s="11">
+        <v>22.5</v>
       </c>
       <c r="F150" s="1">
         <f t="shared" si="0"/>
@@ -6507,7 +6394,7 @@
         <v>2.2453409175959892E-4</v>
       </c>
     </row>
-    <row r="151" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="str">
         <f>'Summary Qty'!A151</f>
         <v>CrownCem</v>
@@ -6524,9 +6411,8 @@
         <f>'Summary Qty'!N151</f>
         <v>0</v>
       </c>
-      <c r="E151" s="1">
-        <f>'Summary Qty'!O151</f>
-        <v>24</v>
+      <c r="E151" s="11">
+        <v>37.5</v>
       </c>
       <c r="F151" s="1">
         <f t="shared" si="0"/>
@@ -6544,7 +6430,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="152" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="str">
         <f>'Summary Qty'!A152</f>
         <v>Rev</v>
@@ -6561,9 +6447,8 @@
         <f>'Summary Qty'!N152</f>
         <v>0</v>
       </c>
-      <c r="E152" s="1">
-        <f>'Summary Qty'!O152</f>
-        <v>46</v>
+      <c r="E152" s="11">
+        <v>22.5</v>
       </c>
       <c r="F152" s="1">
         <f t="shared" si="0"/>
@@ -6581,7 +6466,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="153" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="str">
         <f>'Summary Qty'!A153</f>
         <v>Spl Ins</v>
@@ -6598,9 +6483,8 @@
         <f>'Summary Qty'!N153</f>
         <v>0</v>
       </c>
-      <c r="E153" s="1">
-        <f>'Summary Qty'!O153</f>
-        <v>29</v>
+      <c r="E153" s="11">
+        <v>25</v>
       </c>
       <c r="F153" s="1">
         <f t="shared" si="0"/>
@@ -6618,7 +6502,7 @@
         <v>7.4844697253199639E-5</v>
       </c>
     </row>
-    <row r="154" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <f>'Summary Qty'!A154</f>
         <v>18</v>
@@ -6635,9 +6519,8 @@
         <f>'Summary Qty'!N154</f>
         <v>109.175</v>
       </c>
-      <c r="E154" s="1">
-        <f>'Summary Qty'!O154</f>
-        <v>35</v>
+      <c r="E154" s="11">
+        <v>15</v>
       </c>
       <c r="F154" s="1">
         <f t="shared" si="0"/>
@@ -6655,7 +6538,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="155" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="str">
         <f>'Summary Qty'!A155</f>
         <v>Add LA</v>
@@ -6672,9 +6555,8 @@
         <f>'Summary Qty'!N155</f>
         <v>52.5</v>
       </c>
-      <c r="E155" s="1">
-        <f>'Summary Qty'!O155</f>
-        <v>28</v>
+      <c r="E155" s="11">
+        <v>17.37</v>
       </c>
       <c r="F155" s="1">
         <f t="shared" si="0"/>
@@ -6692,7 +6574,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="156" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="str">
         <f>'Summary Qty'!A156</f>
         <v>InvisR</v>
@@ -6709,9 +6591,8 @@
         <f>'Summary Qty'!N156</f>
         <v>0</v>
       </c>
-      <c r="E156" s="1">
-        <f>'Summary Qty'!O156</f>
-        <v>44</v>
+      <c r="E156" s="11">
+        <v>17.37</v>
       </c>
       <c r="F156" s="1">
         <f t="shared" si="0"/>
@@ -6729,7 +6610,7 @@
         <v>2.4948232417733209E-4</v>
       </c>
     </row>
-    <row r="157" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <f>'Summary Qty'!A157</f>
         <v>245</v>
@@ -6746,9 +6627,8 @@
         <f>'Summary Qty'!N157</f>
         <v>86.6</v>
       </c>
-      <c r="E157" s="1">
-        <f>'Summary Qty'!O157</f>
-        <v>16</v>
+      <c r="E157" s="12">
+        <v>30</v>
       </c>
       <c r="F157" s="1">
         <f t="shared" si="0"/>
@@ -6766,7 +6646,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <f>'Summary Qty'!A158</f>
         <v>451</v>
@@ -6783,9 +6663,8 @@
         <f>'Summary Qty'!N158</f>
         <v>670</v>
       </c>
-      <c r="E158" s="1">
-        <f>'Summary Qty'!O158</f>
-        <v>39</v>
+      <c r="E158" s="12">
+        <v>30</v>
       </c>
       <c r="F158" s="1">
         <f t="shared" si="0"/>
@@ -6803,7 +6682,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="159" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <f>'Summary Qty'!A159</f>
         <v>88535</v>
@@ -6820,9 +6699,8 @@
         <f>'Summary Qty'!N159</f>
         <v>254.75</v>
       </c>
-      <c r="E159" s="1">
-        <f>'Summary Qty'!O159</f>
-        <v>53</v>
+      <c r="E159" s="11">
+        <v>31.52</v>
       </c>
       <c r="F159" s="1">
         <f t="shared" si="0"/>
@@ -6840,7 +6718,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="160" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <f>'Summary Qty'!A160</f>
         <v>632</v>
@@ -6857,9 +6735,8 @@
         <f>'Summary Qty'!N160</f>
         <v>256</v>
       </c>
-      <c r="E160" s="1">
-        <f>'Summary Qty'!O160</f>
-        <v>55</v>
+      <c r="E160" s="11">
+        <v>15</v>
       </c>
       <c r="F160" s="1">
         <f t="shared" si="0"/>
@@ -6877,7 +6754,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="161" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <f>'Summary Qty'!A161</f>
         <v>658</v>
@@ -6894,9 +6771,8 @@
         <f>'Summary Qty'!N161</f>
         <v>263</v>
       </c>
-      <c r="E161" s="1">
-        <f>'Summary Qty'!O161</f>
-        <v>35</v>
+      <c r="E161" s="12">
+        <v>30</v>
       </c>
       <c r="F161" s="1">
         <f t="shared" si="0"/>
@@ -6914,7 +6790,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="162" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <f>'Summary Qty'!A162</f>
         <v>88522</v>
@@ -6931,9 +6807,8 @@
         <f>'Summary Qty'!N162</f>
         <v>143.80000000000001</v>
       </c>
-      <c r="E162" s="1">
-        <f>'Summary Qty'!O162</f>
-        <v>58</v>
+      <c r="E162" s="12">
+        <v>25</v>
       </c>
       <c r="F162" s="1">
         <f t="shared" si="0"/>
@@ -6951,7 +6826,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="163" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="str">
         <f>'Summary Qty'!A163</f>
         <v>Dr Invis Cons</v>
@@ -6968,9 +6843,8 @@
         <f>'Summary Qty'!N163</f>
         <v>0</v>
       </c>
-      <c r="E163" s="1">
-        <f>'Summary Qty'!O163</f>
-        <v>43</v>
+      <c r="E163" s="11">
+        <v>17.37</v>
       </c>
       <c r="F163" s="1">
         <f t="shared" si="0"/>
@@ -6988,7 +6862,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="164" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="str">
         <f>'Summary Qty'!A164</f>
         <v>FIC</v>
@@ -7005,9 +6879,8 @@
         <f>'Summary Qty'!N164</f>
         <v>0</v>
       </c>
-      <c r="E164" s="1">
-        <f>'Summary Qty'!O164</f>
-        <v>47</v>
+      <c r="E164" s="11">
+        <v>17.37</v>
       </c>
       <c r="F164" s="1">
         <f t="shared" si="0"/>
@@ -7025,7 +6898,7 @@
         <v>4.9896464835466422E-5</v>
       </c>
     </row>
-    <row r="165" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <f>'Summary Qty'!A165</f>
         <v>281</v>
@@ -7042,9 +6915,8 @@
         <f>'Summary Qty'!N165</f>
         <v>420</v>
       </c>
-      <c r="E165" s="1">
-        <f>'Summary Qty'!O165</f>
-        <v>15</v>
+      <c r="E165" s="11">
+        <v>26.43</v>
       </c>
       <c r="F165" s="1">
         <f t="shared" si="0"/>
@@ -7062,7 +6934,7 @@
         <v>2.4948232417733211E-5</v>
       </c>
     </row>
-    <row r="166" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <f>'Summary Qty'!A166</f>
         <v>618</v>
@@ -7079,9 +6951,8 @@
         <f>'Summary Qty'!N166</f>
         <v>0</v>
       </c>
-      <c r="E166" s="1">
-        <f>'Summary Qty'!O166</f>
-        <v>0</v>
+      <c r="E166" s="11">
+        <v>25</v>
       </c>
       <c r="F166" s="1">
         <f t="shared" si="0"/>
@@ -7117,9 +6988,7 @@
   </sheetPr>
   <dimension ref="A1:O616"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>